<commit_message>
o Fixed Issue 2, renderig of negative clock values properly. o other comments added
</commit_message>
<xml_diff>
--- a/waveforms__template.xlsx
+++ b/waveforms__template.xlsx
@@ -1110,7 +1110,40 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="71">
+  <dxfs count="74">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2404,7 +2437,7 @@
   <dimension ref="A1:Y66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2476,96 +2509,96 @@
         <v>7</v>
       </c>
       <c r="B3" s="9">
+        <v>-1</v>
+      </c>
+      <c r="C3" s="9">
+        <f t="shared" ref="C3:O5" si="0">B3+1</f>
         <v>0</v>
       </c>
-      <c r="C3" s="9">
-        <f>B3+1</f>
-        <v>1</v>
-      </c>
       <c r="D3" s="9">
-        <f t="shared" ref="D3:O4" si="0">C3+1</f>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E3" s="9">
+        <f t="shared" ref="D3:F5" si="1">D3+1</f>
         <v>2</v>
       </c>
-      <c r="E3" s="9">
+      <c r="F3" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F3" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
       <c r="G3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="H3" s="6">
         <f>F3+9</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" s="9">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J3" s="9">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="L3" s="9">
         <f>J3+1</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M3" s="9">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N3" s="9">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O3" s="9">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="Q3" s="9">
         <f>I3+9</f>
+        <v>22</v>
+      </c>
+      <c r="R3" s="6">
+        <f t="shared" ref="R3:Y3" si="2">Q3+1</f>
         <v>23</v>
       </c>
-      <c r="R3" s="6">
-        <f t="shared" ref="R3:Y3" si="1">Q3+1</f>
+      <c r="S3" s="6">
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="S3" s="6">
-        <f t="shared" si="1"/>
+      <c r="T3" s="6">
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="T3" s="6">
-        <f t="shared" si="1"/>
+      <c r="U3" s="6">
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="U3" s="6">
-        <f t="shared" si="1"/>
+      <c r="V3" s="6">
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="V3" s="6">
-        <f t="shared" si="1"/>
+      <c r="W3" s="6">
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="W3" s="6">
-        <f t="shared" si="1"/>
+      <c r="X3" s="6">
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="X3" s="6">
-        <f t="shared" si="1"/>
+      <c r="Y3" s="6">
+        <f t="shared" si="2"/>
         <v>30</v>
-      </c>
-      <c r="Y3" s="6">
-        <f t="shared" si="1"/>
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
@@ -2573,96 +2606,96 @@
         <v>9</v>
       </c>
       <c r="B4" s="9">
+        <v>-1</v>
+      </c>
+      <c r="C4" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C4" s="9">
-        <f>B4+1</f>
-        <v>1</v>
-      </c>
       <c r="D4" s="9">
-        <f t="shared" ref="D4:F5" si="2">C4+1</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="E4" s="9">
-        <f t="shared" si="2"/>
+      <c r="F4" s="9">
+        <f t="shared" si="1"/>
         <v>3</v>
-      </c>
-      <c r="F4" s="9">
-        <f t="shared" si="2"/>
-        <v>4</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="H4" s="6">
         <f>F4+9</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="6">
         <f>H4+1</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J4" s="6">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="L4" s="9">
         <f>J4+1</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M4" s="6">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N4" s="6">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O4" s="6">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="Q4" s="9">
         <f>O4+3</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R4" s="6">
         <f>Q4+1</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S4" s="6">
         <f t="shared" ref="S4:Y5" si="3">R4+1</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T4" s="6">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U4" s="6">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="V4" s="6">
         <f t="shared" si="3"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W4" s="6">
         <f t="shared" si="3"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X4" s="6">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y4" s="6">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
@@ -2670,97 +2703,97 @@
         <v>8</v>
       </c>
       <c r="B5" s="9">
+        <v>-1</v>
+      </c>
+      <c r="C5" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C5" s="9">
-        <f>B5+1</f>
-        <v>1</v>
-      </c>
       <c r="D5" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="9">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="E5" s="9">
-        <f t="shared" si="2"/>
+      <c r="F5" s="9">
+        <f t="shared" si="1"/>
         <v>3</v>
-      </c>
-      <c r="F5" s="9">
-        <f t="shared" si="2"/>
-        <v>4</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="6">
         <f>F5+9</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" s="6">
         <f>H5+1</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J5" s="6">
         <f t="shared" ref="J5" si="4">I5+1</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K5" s="6">
         <f t="shared" ref="K5" si="5">J5+1</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" ref="L5" si="6">K5+1</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M5" s="6">
         <f t="shared" ref="M5" si="7">L5+1</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N5" s="6">
         <f t="shared" ref="N5" si="8">M5+1</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O5" s="6">
         <f t="shared" ref="O5" si="9">N5+1</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>1</v>
       </c>
       <c r="Q5" s="9">
         <f>O5+3</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R5" s="6">
         <f>Q5+1</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S5" s="6">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="T5" s="6">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U5" s="6">
         <f t="shared" si="3"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V5" s="6">
         <f t="shared" si="3"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W5" s="6">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X5" s="6">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Y5" s="6">
         <f t="shared" si="3"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
@@ -4400,358 +4433,358 @@
   <mergeCells count="1">
     <mergeCell ref="B1:Y1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A47:A52 A56:B56 A15:F21 J14 A12:B14 D13:F13 E14:F14 A22:D22 F22 A57:A63 I44:L44 J18 L18:M18 I20:O20 O14 O22 J15:N15 A11:F11 L4 A4:F4 P4:P7 N11:O13 L11:L14 G4:G7 P9 I8:P8 I10:P10 G9 G11:G21 I22:M22 O23:Q25 K23:L25 J17:N17 K16:L16 K21:L21 S23:V25 N21:O21 L19 F12 C12:D12 H16:I16 H19:I19 H21:I21 A23:H25 O16 O19 P11 I11:J12 C47:XFD52 C61:XFD63 A45:XFD46 N44:XFD44 A2:XFD2 I43:XFD43 Q4:XFD10 P12:XFD22 D57:XFD60 X23:XFD25 R11:XFD11 A53:XFD55 A1:B1 Z1:XFD1 A43:G44 A3:G3 I3:XFD3 A64:XFD1048576">
-    <cfRule type="expression" dxfId="70" priority="124">
+  <conditionalFormatting sqref="A47:A52 A56:B56 A15:F21 J14 A12:B14 D13:F13 E14:F14 A22:D22 F22 A57:A63 I44:L44 J18 L18:M18 I20:O20 O14 O22 J15:N15 A11:F11 L4 A4:B4 P4:P7 N11:O13 L11:L14 G4:G7 P9 I8:P8 I10:P10 G9 G11:G21 I22:M22 O23:Q25 K23:L25 J17:N17 K16:L16 K21:L21 S23:V25 N21:O21 L19 F12 C12:D12 H16:I16 H19:I19 H21:I21 A23:H25 O16 O19 P11 I11:J12 C47:XFD52 C61:XFD63 A45:XFD46 N44:XFD44 A2:XFD2 I43:XFD43 Q4:XFD10 P12:XFD22 D57:XFD60 X23:XFD25 R11:XFD11 A53:XFD55 A1:B1 Z1:XFD1 A43:G44 I3:XFD3 A64:XFD1048576 A3:G3 D4:F4 C4:C5">
+    <cfRule type="expression" dxfId="73" priority="124">
       <formula>$A1="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:XFD56">
-    <cfRule type="expression" dxfId="69" priority="126">
+    <cfRule type="expression" dxfId="72" priority="126">
       <formula>#REF!="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:K14">
-    <cfRule type="expression" dxfId="68" priority="120">
+    <cfRule type="expression" dxfId="71" priority="120">
       <formula>$A13="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="expression" dxfId="67" priority="103">
+    <cfRule type="expression" dxfId="70" priority="103">
       <formula>$A13="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13:I14">
-    <cfRule type="expression" dxfId="66" priority="102">
+    <cfRule type="expression" dxfId="69" priority="102">
       <formula>$A13="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="expression" dxfId="65" priority="93">
+    <cfRule type="expression" dxfId="68" priority="93">
       <formula>$A12="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="64" priority="92">
+    <cfRule type="expression" dxfId="67" priority="92">
       <formula>$A14="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="expression" dxfId="63" priority="91">
+    <cfRule type="expression" dxfId="66" priority="91">
       <formula>$A22="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="expression" dxfId="62" priority="83">
+    <cfRule type="expression" dxfId="65" priority="83">
       <formula>$A12="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M44">
-    <cfRule type="expression" dxfId="61" priority="77">
+    <cfRule type="expression" dxfId="64" priority="77">
       <formula>$A44="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12">
-    <cfRule type="expression" dxfId="60" priority="76">
+    <cfRule type="expression" dxfId="63" priority="76">
       <formula>$A12="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="59" priority="75">
+    <cfRule type="expression" dxfId="62" priority="75">
       <formula>$A14="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="expression" dxfId="58" priority="73">
+    <cfRule type="expression" dxfId="61" priority="73">
       <formula>$A14="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="expression" dxfId="57" priority="72">
+    <cfRule type="expression" dxfId="60" priority="72">
       <formula>$A22="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="expression" dxfId="56" priority="65">
+    <cfRule type="expression" dxfId="59" priority="65">
       <formula>$A44="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18:K19">
-    <cfRule type="expression" dxfId="55" priority="61">
+    <cfRule type="expression" dxfId="58" priority="61">
       <formula>$A18="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14">
-    <cfRule type="expression" dxfId="54" priority="59">
+    <cfRule type="expression" dxfId="57" priority="59">
       <formula>$A14="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:N19">
-    <cfRule type="expression" dxfId="53" priority="58">
+    <cfRule type="expression" dxfId="56" priority="58">
       <formula>$A18="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22">
-    <cfRule type="expression" dxfId="52" priority="55">
+    <cfRule type="expression" dxfId="55" priority="55">
       <formula>$A22="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14">
-    <cfRule type="expression" dxfId="51" priority="53">
+    <cfRule type="expression" dxfId="54" priority="53">
       <formula>$A14="M:"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:F10 G8 G10">
-    <cfRule type="expression" dxfId="50" priority="52">
+  <conditionalFormatting sqref="A6:F10 G8 G10 A5:B5 D5:F5">
+    <cfRule type="expression" dxfId="53" priority="52">
       <formula>$A5="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="49" priority="51">
+    <cfRule type="expression" dxfId="52" priority="51">
       <formula>$A8="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="48" priority="50">
+    <cfRule type="expression" dxfId="51" priority="50">
       <formula>$A10="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:I25">
-    <cfRule type="expression" dxfId="47" priority="48">
+    <cfRule type="expression" dxfId="50" priority="48">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M23:M25">
-    <cfRule type="expression" dxfId="46" priority="47">
+    <cfRule type="expression" dxfId="49" priority="47">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16">
-    <cfRule type="expression" dxfId="45" priority="46">
+    <cfRule type="expression" dxfId="48" priority="46">
       <formula>$A16="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21">
-    <cfRule type="expression" dxfId="44" priority="45">
+    <cfRule type="expression" dxfId="47" priority="45">
       <formula>$A21="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16">
-    <cfRule type="expression" dxfId="43" priority="44">
+    <cfRule type="expression" dxfId="46" priority="44">
       <formula>$A16="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M21">
-    <cfRule type="expression" dxfId="42" priority="43">
+    <cfRule type="expression" dxfId="45" priority="43">
       <formula>$A21="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M19">
-    <cfRule type="expression" dxfId="41" priority="42">
+    <cfRule type="expression" dxfId="44" priority="42">
       <formula>$A19="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M16">
-    <cfRule type="expression" dxfId="40" priority="41">
+    <cfRule type="expression" dxfId="43" priority="41">
       <formula>$A16="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19">
-    <cfRule type="expression" dxfId="39" priority="40">
+    <cfRule type="expression" dxfId="42" priority="40">
       <formula>$A19="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23:J25">
-    <cfRule type="expression" dxfId="38" priority="39">
+    <cfRule type="expression" dxfId="41" priority="39">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N23:N25">
-    <cfRule type="expression" dxfId="37" priority="38">
+    <cfRule type="expression" dxfId="40" priority="38">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W23:W25">
-    <cfRule type="expression" dxfId="36" priority="37">
+    <cfRule type="expression" dxfId="39" priority="37">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="expression" dxfId="35" priority="36">
+    <cfRule type="expression" dxfId="38" priority="36">
       <formula>$A12="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R23:R25">
-    <cfRule type="expression" dxfId="34" priority="35">
+    <cfRule type="expression" dxfId="37" priority="35">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:F40 J33 A31:B33 D32:F32 E33:F33 A41:D41 F41 J37 L37:M37 I39:O39 O33 O41 J34:N34 A30:F30 P26 N30:O32 L30:L33 G26 P28 I27:P27 I29:P29 G28 G30:G40 I41:M41 O42:Q42 K42:L42 J36:N36 K35:L35 K40:L40 S42:V42 N40:O40 L38 F31 C31:D31 H35:I35 H38:I38 H40:I40 A42:H42 O35 O38 P30 I30:J31 Q26:XFD29 P31:XFD41 X42:XFD42 R30:XFD30">
-    <cfRule type="expression" dxfId="33" priority="34">
+    <cfRule type="expression" dxfId="36" priority="34">
       <formula>$A26="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:K33">
-    <cfRule type="expression" dxfId="32" priority="33">
+    <cfRule type="expression" dxfId="35" priority="33">
       <formula>$A32="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32">
-    <cfRule type="expression" dxfId="31" priority="32">
+    <cfRule type="expression" dxfId="34" priority="32">
       <formula>$A32="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32:I33">
-    <cfRule type="expression" dxfId="30" priority="31">
+    <cfRule type="expression" dxfId="33" priority="31">
       <formula>$A32="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="expression" dxfId="29" priority="30">
+    <cfRule type="expression" dxfId="32" priority="30">
       <formula>$A31="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33">
-    <cfRule type="expression" dxfId="28" priority="29">
+    <cfRule type="expression" dxfId="31" priority="29">
       <formula>$A33="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="expression" dxfId="27" priority="28">
+    <cfRule type="expression" dxfId="30" priority="28">
       <formula>$A41="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="expression" dxfId="26" priority="27">
+    <cfRule type="expression" dxfId="29" priority="27">
       <formula>$A31="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M31">
-    <cfRule type="expression" dxfId="25" priority="26">
+    <cfRule type="expression" dxfId="28" priority="26">
       <formula>$A31="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="expression" dxfId="24" priority="25">
+    <cfRule type="expression" dxfId="27" priority="25">
       <formula>$A33="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="expression" dxfId="23" priority="24">
+    <cfRule type="expression" dxfId="26" priority="24">
       <formula>$A33="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="expression" dxfId="22" priority="23">
+    <cfRule type="expression" dxfId="25" priority="23">
       <formula>$A41="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K37:K38">
-    <cfRule type="expression" dxfId="21" priority="22">
+    <cfRule type="expression" dxfId="24" priority="22">
       <formula>$A37="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M33">
-    <cfRule type="expression" dxfId="20" priority="21">
+    <cfRule type="expression" dxfId="23" priority="21">
       <formula>$A33="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N37:N38">
-    <cfRule type="expression" dxfId="19" priority="20">
+    <cfRule type="expression" dxfId="22" priority="20">
       <formula>$A37="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N41">
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="21" priority="19">
       <formula>$A41="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N33">
-    <cfRule type="expression" dxfId="17" priority="18">
+    <cfRule type="expression" dxfId="20" priority="18">
       <formula>$A33="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:F29 G27 G29">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="19" priority="17">
       <formula>$A26="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="18" priority="16">
       <formula>$A27="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="17" priority="15">
       <formula>$A29="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I42">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="16" priority="14">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M42">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="15" priority="13">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J35">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="14" priority="12">
       <formula>$A35="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J40">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="13" priority="11">
       <formula>$A40="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N35">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="12" priority="10">
       <formula>$A35="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M40">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="11" priority="9">
       <formula>$A40="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M38">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="10" priority="8">
       <formula>$A38="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M35">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="9" priority="7">
       <formula>$A35="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>$A38="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N42">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W42">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$A31="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R42">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
o removed footer variable control of Notes: o added notes oncitnuation with sublists
</commit_message>
<xml_diff>
--- a/waveforms__template.xlsx
+++ b/waveforms__template.xlsx
@@ -173,6 +173,33 @@
 o For legible waveforms which fit into an A4 landscape page, 32 cycles are reccomended. 
 O The number of cycles can be doubles by manually changing the scale factor in python, from 4 to 2 or 1 to give a maximum of 128 clocks. However, consider readability. 
 o It is reccomended to use waveform breaks to illustrate lengthy scenarios.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nair Ajayan (IFGB ATV MCD TCD AM):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+negative clocks
+Should start with n
+ie the format should be Cxx:n&lt;clk_name&gt;
+</t>
         </r>
       </text>
     </comment>
@@ -420,7 +447,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="A54" authorId="0">
+    <comment ref="B49" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nair Ajayan (IFGB ATV MCD TCD AM):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+W/o Label node the note is considered  a continulation if marked ith NOTE
+:
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A57" authorId="0">
       <text>
         <r>
           <rPr>
@@ -446,7 +499,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A56" authorId="0">
+    <comment ref="A59" authorId="0">
       <text>
         <r>
           <rPr>
@@ -541,7 +594,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="70">
   <si>
     <t>x</t>
   </si>
@@ -564,9 +617,6 @@
     <t>u</t>
   </si>
   <si>
-    <t>C25:clk_b</t>
-  </si>
-  <si>
     <t>C75:clk_c</t>
   </si>
   <si>
@@ -742,6 +792,18 @@
   </si>
   <si>
     <t>*(A_red+16)[c:r]</t>
+  </si>
+  <si>
+    <t>`+ one more line</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> o Whatever</t>
+  </si>
+  <si>
+    <t>`+ Hahahhann</t>
+  </si>
+  <si>
+    <t>C5:clk_b</t>
   </si>
 </sst>
 </file>
@@ -2239,10 +2301,10 @@
     <row r="5" spans="2:3" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="33" t="s">
         <v>51</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
@@ -2251,23 +2313,23 @@
         <v>Index_nt</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="28" t="s">
         <v>54</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="28" t="s">
         <v>56</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.2">
@@ -2434,10 +2496,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:Y66"/>
+  <dimension ref="A1:Y69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2448,10 +2510,10 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" s="35"/>
       <c r="D1" s="35"/>
@@ -2506,7 +2568,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="B3" s="9">
         <v>-1</v>
@@ -2543,7 +2605,7 @@
         <v>14</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L3" s="9">
         <f>J3+1</f>
@@ -2603,7 +2665,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="9">
         <v>-1</v>
@@ -2640,7 +2702,7 @@
         <v>14</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L4" s="9">
         <f>J4+1</f>
@@ -2700,7 +2762,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="9">
         <v>-1</v>
@@ -2812,7 +2874,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="9">
         <v>0</v>
@@ -2869,7 +2931,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="9">
         <v>0</v>
@@ -2927,16 +2989,16 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>14</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>15</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -2944,10 +3006,10 @@
         <v>1</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L11" s="9"/>
       <c r="N11" s="9" t="s">
@@ -2958,17 +3020,17 @@
         <v>1</v>
       </c>
       <c r="R11" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S11" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T11" s="8"/>
       <c r="X11" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y11" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
@@ -3012,7 +3074,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="9">
         <v>3</v>
@@ -3073,7 +3135,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="9">
         <v>0</v>
@@ -3151,7 +3213,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="9">
         <v>1</v>
@@ -3185,60 +3247,60 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9" t="s">
         <v>1</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N18" s="11" t="s">
         <v>0</v>
       </c>
       <c r="O18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="R18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="S18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P18" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="7" t="s">
+      <c r="U18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="R18" s="7" t="s">
+      <c r="V18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="S18" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="U18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="V18" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="W18" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X18" s="6" t="s">
         <v>6</v>
@@ -3275,7 +3337,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -3339,7 +3401,7 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>6</v>
@@ -3468,7 +3530,7 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26" s="9">
         <v>0</v>
@@ -3525,7 +3587,7 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" s="9">
         <v>0</v>
@@ -3583,16 +3645,16 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>14</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>15</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
@@ -3600,10 +3662,10 @@
         <v>1</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L30" s="9"/>
       <c r="N30" s="9" t="s">
@@ -3614,17 +3676,17 @@
         <v>1</v>
       </c>
       <c r="R30" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S30" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T30" s="8"/>
       <c r="X30" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y30" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
@@ -3668,7 +3730,7 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" s="9">
         <v>3</v>
@@ -3729,7 +3791,7 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" s="9">
         <v>0</v>
@@ -3807,7 +3869,7 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36" s="9">
         <v>1</v>
@@ -3841,7 +3903,7 @@
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>0</v>
@@ -3854,43 +3916,43 @@
         <v>1</v>
       </c>
       <c r="J37" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="K37" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="K37" s="11" t="s">
+      <c r="L37" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="L37" s="10" t="s">
+      <c r="M37" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="M37" s="11" t="s">
-        <v>66</v>
       </c>
       <c r="N37" s="11" t="s">
         <v>0</v>
       </c>
       <c r="O37" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P37" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="R37" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="S37" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P37" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q37" s="7" t="s">
+      <c r="U37" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="R37" s="7" t="s">
+      <c r="V37" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="S37" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="U37" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="V37" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="W37" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X37" s="6" t="s">
         <v>6</v>
@@ -3927,7 +3989,7 @@
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -3991,7 +4053,7 @@
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>6</v>
@@ -4114,13 +4176,13 @@
     </row>
     <row r="45" spans="1:25" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="17" t="s">
         <v>43</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>44</v>
       </c>
       <c r="D45" s="17"/>
       <c r="E45" s="17"/>
@@ -4176,7 +4238,7 @@
         <v>H12&gt;</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.2">
@@ -4188,603 +4250,627 @@
         <v>E12&gt;</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B49" s="6" t="str">
+      <c r="C49" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="6" t="str">
         <f>I42</f>
         <v>I42&gt;</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C52" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H52" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H49" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" s="3" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-    </row>
-    <row r="53" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B53" s="19" t="s">
+    </row>
+    <row r="55" spans="1:8" s="3" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+    </row>
+    <row r="56" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C56" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C53" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" s="3" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+    </row>
+    <row r="57" spans="1:8" s="3" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C54" s="3" t="str">
+      <c r="C57" s="3" t="str">
         <f>A4</f>
         <v>C50:nclk_a</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="22" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="21"/>
-    </row>
-    <row r="56" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="16" t="s">
+    <row r="58" spans="1:8" s="22" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="21"/>
+    </row>
+    <row r="59" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B56" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D56" s="23"/>
-      <c r="E56" s="23"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C57" s="6" t="str">
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60" s="6" t="str">
         <f>H8</f>
         <v>H8&gt;</v>
       </c>
-      <c r="D57" s="6" t="str">
+      <c r="D60" s="6" t="str">
         <f>H10</f>
         <v>H10&gt;</v>
       </c>
-      <c r="E57" s="6" t="str">
+      <c r="E60" s="6" t="str">
         <f>H12</f>
         <v>H12&gt;</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C58" s="6" t="str">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61" s="6" t="str">
         <f>H10</f>
         <v>H10&gt;</v>
       </c>
-      <c r="D58" s="6" t="str">
+      <c r="D61" s="6" t="str">
         <f>N16</f>
         <v>N16&gt;</v>
       </c>
-      <c r="E58" s="6" t="str">
+      <c r="E61" s="6" t="str">
         <f>R23</f>
         <v>R23&gt;</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" s="6" t="str">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C62" s="6" t="str">
         <f>I23</f>
         <v>I23&gt;</v>
       </c>
-      <c r="D59" s="6" t="str">
+      <c r="D62" s="6" t="str">
         <f>M23</f>
         <v>M23&gt;</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="E62" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60" s="6" t="str">
+      <c r="B63" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C63" s="6" t="str">
         <f>J16</f>
         <v>J16&gt;</v>
       </c>
-      <c r="D60" s="6" t="str">
+      <c r="D63" s="6" t="str">
         <f>J19</f>
         <v>J19&gt;</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C61" s="6" t="str">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64" s="6" t="str">
         <f>M23</f>
         <v>M23&gt;</v>
       </c>
-      <c r="D61" s="6" t="str">
+      <c r="D64" s="6" t="str">
         <f>M21</f>
         <v>M21&gt;</v>
       </c>
-      <c r="E61" s="6" t="str">
+      <c r="E64" s="6" t="str">
         <f>M19</f>
         <v>M19&gt;</v>
       </c>
-      <c r="F61" s="6" t="str">
+      <c r="F64" s="6" t="str">
         <f>M16</f>
         <v>M16&gt;</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C62" s="6" t="str">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C65" s="6" t="str">
         <f>J16</f>
         <v>J16&gt;</v>
       </c>
-      <c r="D62" s="6" t="str">
+      <c r="D65" s="6" t="str">
         <f>J19</f>
         <v>J19&gt;</v>
       </c>
-      <c r="E62" s="6" t="str">
+      <c r="E65" s="6" t="str">
         <f>J21</f>
         <v>J21&gt;</v>
       </c>
-      <c r="F62" s="6" t="str">
+      <c r="F65" s="6" t="str">
         <f>J23</f>
         <v>J23&gt;</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C63" s="6" t="str">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C66" s="6" t="str">
         <f>N23</f>
         <v>N23&gt;</v>
       </c>
-      <c r="D63" s="6" t="str">
+      <c r="D66" s="6" t="str">
         <f>R23</f>
         <v>R23&gt;</v>
       </c>
-      <c r="E63" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C64" s="6" t="str">
+      <c r="E66" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C67" s="6" t="str">
         <f>R23</f>
         <v>R23&gt;</v>
       </c>
-      <c r="D64" s="6" t="str">
+      <c r="D67" s="6" t="str">
         <f>W23</f>
         <v>W23&gt;</v>
       </c>
-      <c r="E64" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
+      <c r="E67" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B65" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C65" s="6" t="str">
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C68" s="6" t="str">
         <f>R23</f>
         <v>R23&gt;</v>
       </c>
-      <c r="D65" s="6" t="str">
+      <c r="D68" s="6" t="str">
         <f>W23</f>
         <v>W23&gt;</v>
       </c>
-      <c r="E65" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="3" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
+      <c r="E68" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="3" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="B1:Y1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A47:A52 A56:B56 A15:F21 J14 A12:B14 D13:F13 E14:F14 A22:D22 F22 A57:A63 I44:L44 J18 L18:M18 I20:O20 O14 O22 J15:N15 A11:F11 L4 A4:B4 P4:P7 N11:O13 L11:L14 G4:G7 P9 I8:P8 I10:P10 G9 G11:G21 I22:M22 O23:Q25 K23:L25 J17:N17 K16:L16 K21:L21 S23:V25 N21:O21 L19 F12 C12:D12 H16:I16 H19:I19 H21:I21 A23:H25 O16 O19 P11 I11:J12 C47:XFD52 C61:XFD63 A45:XFD46 N44:XFD44 A2:XFD2 I43:XFD43 Q4:XFD10 P12:XFD22 D57:XFD60 X23:XFD25 R11:XFD11 A53:XFD55 A1:B1 Z1:XFD1 A43:G44 I3:XFD3 A64:XFD1048576 A3:G3 D4:F4 C4:C5">
-    <cfRule type="expression" dxfId="73" priority="124">
+  <conditionalFormatting sqref="A47:A55 A59:B59 A15:F21 J14 A12:B14 D13:F13 E14:F14 A22:D22 F22 A60:A66 I44:L44 J18 L18:M18 I20:O20 O14 O22 J15:N15 A11:F11 L4 A4:B4 P4:P7 N11:O13 L11:L14 G4:G7 P9 I8:P8 I10:P10 G9 G11:G21 I22:M22 O23:Q25 K23:L25 J17:N17 K16:L16 K21:L21 S23:V25 N21:O21 L19 F12 C12:D12 H16:I16 H19:I19 H21:I21 A23:H25 O16 O19 P11 I11:J12 C47:XFD55 C64:XFD66 A45:XFD46 N44:XFD44 A2:XFD2 I43:XFD43 Q4:XFD10 P12:XFD22 D60:XFD63 X23:XFD25 R11:XFD11 A56:XFD58 A1:B1 Z1:XFD1 A43:G44 I3:XFD3 A3:G3 D4:F4 C4:C5 A67:XFD1048576">
+    <cfRule type="expression" dxfId="70" priority="124">
       <formula>$A1="M:"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56:XFD56">
-    <cfRule type="expression" dxfId="72" priority="126">
+  <conditionalFormatting sqref="C59:XFD59">
+    <cfRule type="expression" dxfId="69" priority="126">
       <formula>#REF!="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:K14">
-    <cfRule type="expression" dxfId="71" priority="120">
+    <cfRule type="expression" dxfId="68" priority="120">
       <formula>$A13="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="expression" dxfId="70" priority="103">
+    <cfRule type="expression" dxfId="67" priority="103">
       <formula>$A13="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13:I14">
-    <cfRule type="expression" dxfId="69" priority="102">
+    <cfRule type="expression" dxfId="66" priority="102">
       <formula>$A13="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="expression" dxfId="68" priority="93">
+    <cfRule type="expression" dxfId="65" priority="93">
       <formula>$A12="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="67" priority="92">
+    <cfRule type="expression" dxfId="64" priority="92">
       <formula>$A14="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="expression" dxfId="66" priority="91">
+    <cfRule type="expression" dxfId="63" priority="91">
       <formula>$A22="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="expression" dxfId="65" priority="83">
+    <cfRule type="expression" dxfId="62" priority="83">
       <formula>$A12="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M44">
-    <cfRule type="expression" dxfId="64" priority="77">
+    <cfRule type="expression" dxfId="61" priority="77">
       <formula>$A44="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12">
-    <cfRule type="expression" dxfId="63" priority="76">
+    <cfRule type="expression" dxfId="60" priority="76">
       <formula>$A12="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="62" priority="75">
+    <cfRule type="expression" dxfId="59" priority="75">
       <formula>$A14="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="expression" dxfId="61" priority="73">
+    <cfRule type="expression" dxfId="58" priority="73">
       <formula>$A14="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="expression" dxfId="60" priority="72">
+    <cfRule type="expression" dxfId="57" priority="72">
       <formula>$A22="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="expression" dxfId="59" priority="65">
+    <cfRule type="expression" dxfId="56" priority="65">
       <formula>$A44="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18:K19">
-    <cfRule type="expression" dxfId="58" priority="61">
+    <cfRule type="expression" dxfId="55" priority="61">
       <formula>$A18="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14">
-    <cfRule type="expression" dxfId="57" priority="59">
+    <cfRule type="expression" dxfId="54" priority="59">
       <formula>$A14="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:N19">
-    <cfRule type="expression" dxfId="56" priority="58">
+    <cfRule type="expression" dxfId="53" priority="58">
       <formula>$A18="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22">
-    <cfRule type="expression" dxfId="55" priority="55">
+    <cfRule type="expression" dxfId="52" priority="55">
       <formula>$A22="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14">
-    <cfRule type="expression" dxfId="54" priority="53">
+    <cfRule type="expression" dxfId="51" priority="53">
       <formula>$A14="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:F10 G8 G10 A5:B5 D5:F5">
-    <cfRule type="expression" dxfId="53" priority="52">
+    <cfRule type="expression" dxfId="50" priority="52">
       <formula>$A5="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="52" priority="51">
+    <cfRule type="expression" dxfId="49" priority="51">
       <formula>$A8="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="51" priority="50">
+    <cfRule type="expression" dxfId="48" priority="50">
       <formula>$A10="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:I25">
-    <cfRule type="expression" dxfId="50" priority="48">
+    <cfRule type="expression" dxfId="47" priority="48">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M23:M25">
-    <cfRule type="expression" dxfId="49" priority="47">
+    <cfRule type="expression" dxfId="46" priority="47">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16">
-    <cfRule type="expression" dxfId="48" priority="46">
+    <cfRule type="expression" dxfId="45" priority="46">
       <formula>$A16="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21">
-    <cfRule type="expression" dxfId="47" priority="45">
+    <cfRule type="expression" dxfId="44" priority="45">
       <formula>$A21="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16">
-    <cfRule type="expression" dxfId="46" priority="44">
+    <cfRule type="expression" dxfId="43" priority="44">
       <formula>$A16="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M21">
-    <cfRule type="expression" dxfId="45" priority="43">
+    <cfRule type="expression" dxfId="42" priority="43">
       <formula>$A21="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M19">
-    <cfRule type="expression" dxfId="44" priority="42">
+    <cfRule type="expression" dxfId="41" priority="42">
       <formula>$A19="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M16">
-    <cfRule type="expression" dxfId="43" priority="41">
+    <cfRule type="expression" dxfId="40" priority="41">
       <formula>$A16="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19">
-    <cfRule type="expression" dxfId="42" priority="40">
+    <cfRule type="expression" dxfId="39" priority="40">
       <formula>$A19="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23:J25">
-    <cfRule type="expression" dxfId="41" priority="39">
+    <cfRule type="expression" dxfId="38" priority="39">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N23:N25">
-    <cfRule type="expression" dxfId="40" priority="38">
+    <cfRule type="expression" dxfId="37" priority="38">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W23:W25">
-    <cfRule type="expression" dxfId="39" priority="37">
+    <cfRule type="expression" dxfId="36" priority="37">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="expression" dxfId="38" priority="36">
+    <cfRule type="expression" dxfId="35" priority="36">
       <formula>$A12="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R23:R25">
-    <cfRule type="expression" dxfId="37" priority="35">
+    <cfRule type="expression" dxfId="34" priority="35">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:F40 J33 A31:B33 D32:F32 E33:F33 A41:D41 F41 J37 L37:M37 I39:O39 O33 O41 J34:N34 A30:F30 P26 N30:O32 L30:L33 G26 P28 I27:P27 I29:P29 G28 G30:G40 I41:M41 O42:Q42 K42:L42 J36:N36 K35:L35 K40:L40 S42:V42 N40:O40 L38 F31 C31:D31 H35:I35 H38:I38 H40:I40 A42:H42 O35 O38 P30 I30:J31 Q26:XFD29 P31:XFD41 X42:XFD42 R30:XFD30">
-    <cfRule type="expression" dxfId="36" priority="34">
+    <cfRule type="expression" dxfId="33" priority="34">
       <formula>$A26="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:K33">
-    <cfRule type="expression" dxfId="35" priority="33">
+    <cfRule type="expression" dxfId="32" priority="33">
       <formula>$A32="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32">
-    <cfRule type="expression" dxfId="34" priority="32">
+    <cfRule type="expression" dxfId="31" priority="32">
       <formula>$A32="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32:I33">
-    <cfRule type="expression" dxfId="33" priority="31">
+    <cfRule type="expression" dxfId="30" priority="31">
       <formula>$A32="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="expression" dxfId="32" priority="30">
+    <cfRule type="expression" dxfId="29" priority="30">
       <formula>$A31="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33">
-    <cfRule type="expression" dxfId="31" priority="29">
+    <cfRule type="expression" dxfId="28" priority="29">
       <formula>$A33="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="expression" dxfId="30" priority="28">
+    <cfRule type="expression" dxfId="27" priority="28">
       <formula>$A41="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="expression" dxfId="29" priority="27">
+    <cfRule type="expression" dxfId="26" priority="27">
       <formula>$A31="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M31">
-    <cfRule type="expression" dxfId="28" priority="26">
+    <cfRule type="expression" dxfId="25" priority="26">
       <formula>$A31="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="expression" dxfId="27" priority="25">
+    <cfRule type="expression" dxfId="24" priority="25">
       <formula>$A33="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="expression" dxfId="26" priority="24">
+    <cfRule type="expression" dxfId="23" priority="24">
       <formula>$A33="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="expression" dxfId="25" priority="23">
+    <cfRule type="expression" dxfId="22" priority="23">
       <formula>$A41="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K37:K38">
-    <cfRule type="expression" dxfId="24" priority="22">
+    <cfRule type="expression" dxfId="21" priority="22">
       <formula>$A37="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M33">
-    <cfRule type="expression" dxfId="23" priority="21">
+    <cfRule type="expression" dxfId="20" priority="21">
       <formula>$A33="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N37:N38">
-    <cfRule type="expression" dxfId="22" priority="20">
+    <cfRule type="expression" dxfId="19" priority="20">
       <formula>$A37="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N41">
-    <cfRule type="expression" dxfId="21" priority="19">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>$A41="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N33">
-    <cfRule type="expression" dxfId="20" priority="18">
+    <cfRule type="expression" dxfId="17" priority="18">
       <formula>$A33="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:F29 G27 G29">
-    <cfRule type="expression" dxfId="19" priority="17">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>$A26="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="expression" dxfId="18" priority="16">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>$A27="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="expression" dxfId="17" priority="15">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>$A29="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I42">
-    <cfRule type="expression" dxfId="16" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M42">
-    <cfRule type="expression" dxfId="15" priority="13">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J35">
-    <cfRule type="expression" dxfId="14" priority="12">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>$A35="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J40">
-    <cfRule type="expression" dxfId="13" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>$A40="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N35">
-    <cfRule type="expression" dxfId="12" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>$A35="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M40">
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>$A40="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M38">
-    <cfRule type="expression" dxfId="10" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>$A38="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M35">
-    <cfRule type="expression" dxfId="9" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>$A35="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38">
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>$A38="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N42">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W42">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$A31="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R42">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4807,7 +4893,7 @@
   <sheetData>
     <row r="5" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added control of SCALE to worksheet
</commit_message>
<xml_diff>
--- a/waveforms__template.xlsx
+++ b/waveforms__template.xlsx
@@ -21,7 +21,36 @@
     <author>Nair Ajayan (IFGB ATV MCD TCD AM)</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0">
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nair Ajayan (IFGB ATV MCD TCD AM):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Default is 4:
+will override SCALE provided from connand line.
+@4 approx 22-25 clock cycles can be drawn
+Overflow is indicated by a black box in th PDF.
+Halving scales, for example doubles the clocks that can be drawn
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0">
+    <comment ref="C4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="0">
+    <comment ref="G4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="0">
+    <comment ref="K4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -150,7 +179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y3" authorId="0">
+    <comment ref="Y4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -176,7 +205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0">
+    <comment ref="A5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -203,7 +232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K4" authorId="0">
+    <comment ref="K5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -228,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0">
+    <comment ref="A8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -271,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="0">
+    <comment ref="A9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -313,7 +342,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0">
+    <comment ref="A12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -352,7 +381,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0">
+    <comment ref="E13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -388,7 +417,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A46" authorId="0">
+    <comment ref="A47" authorId="0">
       <text>
         <r>
           <rPr>
@@ -402,7 +431,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B47" authorId="0">
+    <comment ref="B48" authorId="0">
       <text>
         <r>
           <rPr>
@@ -447,7 +476,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B49" authorId="0">
+    <comment ref="B50" authorId="0">
       <text>
         <r>
           <rPr>
@@ -473,7 +502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A57" authorId="0">
+    <comment ref="A58" authorId="0">
       <text>
         <r>
           <rPr>
@@ -499,7 +528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A59" authorId="0">
+    <comment ref="A60" authorId="0">
       <text>
         <r>
           <rPr>
@@ -594,7 +623,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="71">
   <si>
     <t>x</t>
   </si>
@@ -804,6 +833,9 @@
   </si>
   <si>
     <t>C5:clk_b</t>
+  </si>
+  <si>
+    <t>:SCALE:</t>
   </si>
 </sst>
 </file>
@@ -1172,40 +1204,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="74">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="71">
     <dxf>
       <font>
         <strike val="0"/>
@@ -2496,11 +2495,9 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:Y69"/>
+  <dimension ref="A1:Y70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2509,181 +2506,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B2" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="9">
-        <v>-1</v>
-      </c>
-      <c r="C3" s="9">
-        <f t="shared" ref="C3:O5" si="0">B3+1</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E3" s="9">
-        <f t="shared" ref="D3:F5" si="1">D3+1</f>
-        <v>2</v>
-      </c>
-      <c r="F3" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="6">
-        <f>F3+9</f>
-        <v>12</v>
-      </c>
-      <c r="I3" s="9">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="J3" s="9">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="9">
-        <f>J3+1</f>
-        <v>15</v>
-      </c>
-      <c r="M3" s="9">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="N3" s="9">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="O3" s="9">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="9">
-        <f>I3+9</f>
-        <v>22</v>
-      </c>
-      <c r="R3" s="6">
-        <f t="shared" ref="R3:Y3" si="2">Q3+1</f>
-        <v>23</v>
-      </c>
-      <c r="S3" s="6">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="T3" s="6">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="U3" s="6">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="V3" s="6">
-        <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="W3" s="6">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="X3" s="6">
-        <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-      <c r="Y3" s="6">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="B4" s="9">
         <v>-1</v>
       </c>
       <c r="C4" s="9">
+        <f t="shared" ref="C4:O6" si="0">B4+1</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D4" s="9">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E4" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D4:F6" si="1">D4+1</f>
         <v>2</v>
       </c>
       <c r="F4" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G4" s="9" t="s">
@@ -2693,30 +2601,30 @@
         <f>F4+9</f>
         <v>12</v>
       </c>
-      <c r="I4" s="6">
-        <f>H4+1</f>
+      <c r="I4" s="9">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="L4" s="9">
         <f>J4+1</f>
         <v>15</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="9">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="9">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="9">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -2724,45 +2632,45 @@
         <v>1</v>
       </c>
       <c r="Q4" s="9">
-        <f>O4+3</f>
-        <v>21</v>
+        <f>I4+9</f>
+        <v>22</v>
       </c>
       <c r="R4" s="6">
-        <f>Q4+1</f>
-        <v>22</v>
+        <f t="shared" ref="R4:Y4" si="2">Q4+1</f>
+        <v>23</v>
       </c>
       <c r="S4" s="6">
-        <f t="shared" ref="S4:Y5" si="3">R4+1</f>
-        <v>23</v>
+        <f t="shared" si="2"/>
+        <v>24</v>
       </c>
       <c r="T4" s="6">
-        <f t="shared" si="3"/>
-        <v>24</v>
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
       <c r="U4" s="6">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f t="shared" si="2"/>
+        <v>26</v>
       </c>
       <c r="V4" s="6">
-        <f t="shared" si="3"/>
-        <v>26</v>
+        <f t="shared" si="2"/>
+        <v>27</v>
       </c>
       <c r="W4" s="6">
-        <f t="shared" si="3"/>
-        <v>27</v>
+        <f t="shared" si="2"/>
+        <v>28</v>
       </c>
       <c r="X4" s="6">
-        <f t="shared" si="3"/>
-        <v>28</v>
+        <f t="shared" si="2"/>
+        <v>29</v>
       </c>
       <c r="Y4" s="6">
-        <f t="shared" si="3"/>
-        <v>29</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="9">
         <v>-1</v>
@@ -2795,111 +2703,175 @@
         <v>13</v>
       </c>
       <c r="J5" s="6">
-        <f t="shared" ref="J5" si="4">I5+1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="K5" s="6">
-        <f t="shared" ref="K5" si="5">J5+1</f>
+      <c r="K5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="9">
+        <f>J5+1</f>
         <v>15</v>
       </c>
-      <c r="L5" s="6">
-        <f t="shared" ref="L5" si="6">K5+1</f>
+      <c r="M5" s="6">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="M5" s="6">
-        <f t="shared" ref="M5" si="7">L5+1</f>
+      <c r="N5" s="6">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="N5" s="6">
-        <f t="shared" ref="N5" si="8">M5+1</f>
+      <c r="O5" s="6">
+        <f t="shared" si="0"/>
         <v>18</v>
-      </c>
-      <c r="O5" s="6">
-        <f t="shared" ref="O5" si="9">N5+1</f>
-        <v>19</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>1</v>
       </c>
       <c r="Q5" s="9">
         <f>O5+3</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R5" s="6">
         <f>Q5+1</f>
+        <v>22</v>
+      </c>
+      <c r="S5" s="6">
+        <f t="shared" ref="S5:Y6" si="3">R5+1</f>
         <v>23</v>
       </c>
-      <c r="S5" s="6">
+      <c r="T5" s="6">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="T5" s="6">
+      <c r="U5" s="6">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="U5" s="6">
+      <c r="V5" s="6">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="V5" s="6">
+      <c r="W5" s="6">
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="W5" s="6">
+      <c r="X5" s="6">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="X5" s="6">
+      <c r="Y5" s="6">
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="Y5" s="6">
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="9">
+        <v>-1</v>
+      </c>
+      <c r="C6" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E6" s="9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F6" s="9">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6">
+        <f>F6+9</f>
+        <v>12</v>
+      </c>
+      <c r="I6" s="6">
+        <f>H6+1</f>
+        <v>13</v>
+      </c>
+      <c r="J6" s="6">
+        <f t="shared" ref="J6" si="4">I6+1</f>
+        <v>14</v>
+      </c>
+      <c r="K6" s="6">
+        <f t="shared" ref="K6" si="5">J6+1</f>
+        <v>15</v>
+      </c>
+      <c r="L6" s="6">
+        <f t="shared" ref="L6" si="6">K6+1</f>
+        <v>16</v>
+      </c>
+      <c r="M6" s="6">
+        <f t="shared" ref="M6" si="7">L6+1</f>
+        <v>17</v>
+      </c>
+      <c r="N6" s="6">
+        <f t="shared" ref="N6" si="8">M6+1</f>
+        <v>18</v>
+      </c>
+      <c r="O6" s="6">
+        <f t="shared" ref="O6" si="9">N6+1</f>
+        <v>19</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="9">
+        <f>O6+3</f>
+        <v>22</v>
+      </c>
+      <c r="R6" s="6">
+        <f>Q6+1</f>
+        <v>23</v>
+      </c>
+      <c r="S6" s="6">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="T6" s="6">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="U6" s="6">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="V6" s="6">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="W6" s="6">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="X6" s="6">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="Y6" s="6">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="9"/>
-    </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="9">
-        <v>0</v>
-      </c>
+      <c r="B7" s="9"/>
       <c r="C7" s="9"/>
-      <c r="D7" s="9">
-        <v>1</v>
-      </c>
+      <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="6">
-        <v>1</v>
-      </c>
-      <c r="I7" s="6">
-        <v>1</v>
-      </c>
-      <c r="L7" s="6">
-        <v>1</v>
-      </c>
-      <c r="N7" s="6">
-        <v>0</v>
-      </c>
       <c r="P7" s="9" t="s">
         <v>1</v>
       </c>
@@ -2907,197 +2879,195 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="9"/>
+        <v>10</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0</v>
+      </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>H8&gt;</v>
-      </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
+      <c r="G8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="6">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6">
+        <v>1</v>
+      </c>
+      <c r="L8" s="6">
+        <v>1</v>
+      </c>
+      <c r="N8" s="6">
+        <v>0</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="Q8" s="9"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="9">
-        <v>0</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="6">
-        <v>1</v>
-      </c>
-      <c r="I9" s="6">
-        <v>1</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0</v>
-      </c>
-      <c r="M9" s="6">
-        <v>1</v>
-      </c>
-      <c r="N9" s="6">
-        <v>0</v>
-      </c>
-      <c r="P9" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>H9&gt;</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="9"/>
+        <v>11</v>
+      </c>
+      <c r="B10" s="9">
+        <v>0</v>
+      </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>H10&gt;</v>
-      </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
+      <c r="G10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1</v>
+      </c>
+      <c r="I10" s="6">
+        <v>1</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0</v>
+      </c>
+      <c r="M10" s="6">
+        <v>1</v>
+      </c>
+      <c r="N10" s="6">
+        <v>0</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="Q10" s="9"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>H11&gt;</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
       <c r="L11" s="9"/>
-      <c r="N11" s="9" t="s">
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="R11" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="S11" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="T11" s="8"/>
-      <c r="X11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y11" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>E12&gt;</v>
-      </c>
+      <c r="C12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>H12&gt;</v>
-      </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>K12&gt;</v>
+      <c r="I12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="L12" s="9"/>
-      <c r="M12" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>M12&gt;</v>
-      </c>
-      <c r="N12" s="9"/>
+      <c r="N12" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="O12" s="9"/>
       <c r="P12" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
+      <c r="R12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="S12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="T12" s="8"/>
+      <c r="X12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y12" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="9">
         <v>3</v>
       </c>
-      <c r="C13" s="6">
-        <v>3</v>
-      </c>
-      <c r="D13" s="9">
-        <v>5</v>
-      </c>
-      <c r="E13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>E13&gt;</v>
+      </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="I13" s="11">
-        <v>6</v>
-      </c>
-      <c r="J13" s="11">
-        <v>5</v>
-      </c>
-      <c r="K13" s="11"/>
+      <c r="H13" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>H13&gt;</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>K13&gt;</v>
+      </c>
       <c r="L13" s="9"/>
+      <c r="M13" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>M13&gt;</v>
+      </c>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
       <c r="P13" s="9" t="s">
@@ -3106,24 +3076,33 @@
       <c r="Q13" s="9"/>
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
-      <c r="U13" s="8"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="9">
+        <v>3</v>
+      </c>
+      <c r="C14" s="6">
+        <v>3</v>
+      </c>
+      <c r="D14" s="9">
+        <v>5</v>
+      </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="10"/>
+      <c r="I14" s="11">
+        <v>6</v>
+      </c>
+      <c r="J14" s="11">
+        <v>5</v>
+      </c>
       <c r="K14" s="11"/>
       <c r="L14" s="9"/>
-      <c r="M14" s="11"/>
       <c r="N14" s="9"/>
       <c r="O14" s="9"/>
       <c r="P14" s="9" t="s">
@@ -3132,14 +3111,11 @@
       <c r="Q14" s="9"/>
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
+      <c r="U14" s="8"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="9">
-        <v>0</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="9"/>
@@ -3147,364 +3123,371 @@
       <c r="G15" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="J15" s="9">
-        <v>1</v>
-      </c>
-      <c r="K15" s="10">
-        <v>1</v>
-      </c>
-      <c r="L15" s="10">
-        <v>1</v>
-      </c>
-      <c r="M15" s="11">
-        <v>1</v>
-      </c>
-      <c r="N15" s="10">
-        <v>0</v>
-      </c>
-      <c r="O15" s="6">
-        <v>1</v>
-      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
       <c r="P15" s="9" t="s">
         <v>1</v>
       </c>
       <c r="Q15" s="9"/>
-      <c r="R15" s="7">
-        <v>1</v>
-      </c>
-      <c r="S15" s="7">
-        <v>1</v>
-      </c>
-      <c r="X15" s="6">
-        <v>0</v>
-      </c>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0</v>
+      </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>J16&gt;</v>
-      </c>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>M16&gt;</v>
-      </c>
-      <c r="N16" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>N16&gt;</v>
-      </c>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
+      <c r="G16" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="9">
+        <v>1</v>
+      </c>
+      <c r="K16" s="10">
+        <v>1</v>
+      </c>
+      <c r="L16" s="10">
+        <v>1</v>
+      </c>
+      <c r="M16" s="11">
+        <v>1</v>
+      </c>
+      <c r="N16" s="10">
+        <v>0</v>
+      </c>
+      <c r="O16" s="6">
+        <v>1</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="Q16" s="9"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
+      <c r="R16" s="7">
+        <v>1</v>
+      </c>
+      <c r="S16" s="7">
+        <v>1</v>
+      </c>
+      <c r="X16" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="9">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B17" s="9"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>J17&gt;</v>
+      </c>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="10"/>
-      <c r="P17" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="M17" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>M17&gt;</v>
+      </c>
+      <c r="N17" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>N17&gt;</v>
+      </c>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
       <c r="Q17" s="9"/>
       <c r="R17" s="7"/>
-      <c r="S17" s="7">
-        <v>0</v>
-      </c>
-      <c r="T17" s="6">
-        <v>1</v>
-      </c>
-      <c r="X17" s="6">
-        <v>0</v>
-      </c>
+      <c r="S17" s="7"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="B18" s="9">
+        <v>1</v>
       </c>
       <c r="C18" s="11"/>
-      <c r="D18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>38</v>
-      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L18" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="M18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="N18" s="11" t="s">
+      <c r="J18" s="9"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="10"/>
+      <c r="P18" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7">
         <v>0</v>
       </c>
-      <c r="O18" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P18" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="R18" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="S18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="U18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="V18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="W18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="X18" s="6" t="s">
-        <v>6</v>
+      <c r="T18" s="6">
+        <v>1</v>
+      </c>
+      <c r="X18" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N19" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P19" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="U19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="V19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="W19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="X19" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>J19&gt;</v>
-      </c>
-      <c r="K19" s="11"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>M19&gt;</v>
-      </c>
-      <c r="N19" s="11"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
       <c r="I20" s="9"/>
-      <c r="J20" s="9">
-        <v>6</v>
-      </c>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="O20" s="10">
-        <v>5</v>
-      </c>
-      <c r="P20" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="12"/>
-      <c r="S20" s="12"/>
-      <c r="X20" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="J20" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>J20&gt;</v>
+      </c>
+      <c r="K20" s="11"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>M20&gt;</v>
+      </c>
+      <c r="N20" s="11"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
+      <c r="G21" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="I21" s="9"/>
-      <c r="J21" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>J21&gt;</v>
+      <c r="J21" s="9">
+        <v>6</v>
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
-      <c r="M21" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>M21&gt;</v>
-      </c>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="O21" s="10">
+        <v>5</v>
+      </c>
+      <c r="P21" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="Q21" s="10"/>
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
+      <c r="X21" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>6</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="11"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H22" s="9"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
       <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
+      <c r="J22" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>J22&gt;</v>
+      </c>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
-      <c r="M22" s="9">
-        <v>1</v>
-      </c>
-      <c r="N22" s="11">
+      <c r="M22" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>M22&gt;</v>
+      </c>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9">
+        <v>1</v>
+      </c>
+      <c r="N23" s="11">
         <v>0</v>
       </c>
-      <c r="O22" s="10"/>
-      <c r="P22" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="12">
-        <v>1</v>
-      </c>
-      <c r="S22" s="12">
+      <c r="O23" s="10"/>
+      <c r="P23" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="12">
+        <v>1</v>
+      </c>
+      <c r="S23" s="12">
         <v>0</v>
       </c>
-      <c r="W22" s="6">
-        <v>1</v>
-      </c>
-      <c r="X22" s="6">
+      <c r="W23" s="6">
+        <v>1</v>
+      </c>
+      <c r="X23" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>I23&gt;</v>
-      </c>
-      <c r="J23" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>J23&gt;</v>
-      </c>
-      <c r="K23" s="10"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>M23&gt;</v>
-      </c>
-      <c r="N23" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>N23&gt;</v>
-      </c>
-      <c r="O23" s="11"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>R23&gt;</v>
-      </c>
-      <c r="S23" s="7"/>
-      <c r="W23" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>W23&gt;</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="34"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>I24&gt;</v>
+      </c>
+      <c r="J24" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>J24&gt;</v>
+      </c>
+      <c r="K24" s="10"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>M24&gt;</v>
+      </c>
+      <c r="N24" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>N24&gt;</v>
+      </c>
+      <c r="O24" s="11"/>
       <c r="P24" s="10"/>
       <c r="Q24" s="9"/>
-      <c r="R24" s="34"/>
+      <c r="R24" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>R24&gt;</v>
+      </c>
       <c r="S24" s="7"/>
-      <c r="W24" s="34"/>
+      <c r="W24" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>W24&gt;</v>
+      </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
@@ -3529,231 +3512,218 @@
       <c r="W25" s="34"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="9">
-        <v>0</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9">
-        <v>1</v>
-      </c>
+      <c r="A26" s="1"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
-      <c r="G26" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H26" s="6">
-        <v>1</v>
-      </c>
-      <c r="I26" s="6">
-        <v>1</v>
-      </c>
-      <c r="L26" s="6">
-        <v>1</v>
-      </c>
-      <c r="N26" s="6">
-        <v>0</v>
-      </c>
-      <c r="P26" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="34"/>
+      <c r="P26" s="10"/>
       <c r="Q26" s="9"/>
+      <c r="R26" s="34"/>
+      <c r="S26" s="7"/>
+      <c r="W26" s="34"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="9"/>
+        <v>10</v>
+      </c>
+      <c r="B27" s="9">
+        <v>0</v>
+      </c>
       <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
+      <c r="D27" s="9">
+        <v>1</v>
+      </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>H27&gt;</v>
-      </c>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
+      <c r="G27" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27" s="6">
+        <v>1</v>
+      </c>
+      <c r="I27" s="6">
+        <v>1</v>
+      </c>
+      <c r="L27" s="6">
+        <v>1</v>
+      </c>
+      <c r="N27" s="6">
+        <v>0</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="Q27" s="9"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="9">
-        <v>0</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
-      <c r="G28" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H28" s="6">
-        <v>1</v>
-      </c>
-      <c r="I28" s="6">
-        <v>1</v>
-      </c>
-      <c r="J28" s="6">
-        <v>0</v>
-      </c>
-      <c r="M28" s="6">
-        <v>1</v>
-      </c>
-      <c r="N28" s="6">
-        <v>0</v>
-      </c>
-      <c r="P28" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="G28" s="9"/>
+      <c r="H28" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>H28&gt;</v>
+      </c>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
       <c r="Q28" s="9"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="9"/>
+        <v>11</v>
+      </c>
+      <c r="B29" s="9">
+        <v>0</v>
+      </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>H29&gt;</v>
-      </c>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
+      <c r="G29" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="6">
+        <v>1</v>
+      </c>
+      <c r="I29" s="6">
+        <v>1</v>
+      </c>
+      <c r="J29" s="6">
+        <v>0</v>
+      </c>
+      <c r="M29" s="6">
+        <v>1</v>
+      </c>
+      <c r="N29" s="6">
+        <v>0</v>
+      </c>
+      <c r="P29" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="Q29" s="9"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A30" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="A30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J30" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="G30" s="9"/>
+      <c r="H30" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>H30&gt;</v>
+      </c>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
       <c r="L30" s="9"/>
-      <c r="N30" s="9" t="s">
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A31" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="R30" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="S30" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="T30" s="8"/>
-      <c r="X30" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y30" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>E31&gt;</v>
-      </c>
+      <c r="C31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H31" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>H31&gt;</v>
-      </c>
-      <c r="I31" s="9"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>K31&gt;</v>
+      <c r="I31" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="L31" s="9"/>
-      <c r="M31" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>M31&gt;</v>
-      </c>
-      <c r="N31" s="9"/>
+      <c r="N31" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="O31" s="9"/>
       <c r="P31" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
+      <c r="R31" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="S31" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="T31" s="8"/>
+      <c r="X31" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y31" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="9">
         <v>3</v>
       </c>
-      <c r="C32" s="6">
-        <v>3</v>
-      </c>
-      <c r="D32" s="9">
-        <v>5</v>
-      </c>
-      <c r="E32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>E32&gt;</v>
+      </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="I32" s="11">
-        <v>6</v>
-      </c>
-      <c r="J32" s="11">
-        <v>5</v>
-      </c>
-      <c r="K32" s="11"/>
+      <c r="H32" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>H32&gt;</v>
+      </c>
+      <c r="I32" s="9"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>K32&gt;</v>
+      </c>
       <c r="L32" s="9"/>
+      <c r="M32" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>M32&gt;</v>
+      </c>
       <c r="N32" s="9"/>
       <c r="O32" s="9"/>
       <c r="P32" s="9" t="s">
@@ -3762,24 +3732,33 @@
       <c r="Q32" s="9"/>
       <c r="R32" s="7"/>
       <c r="S32" s="7"/>
-      <c r="U32" s="8"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
+      <c r="A33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="9">
+        <v>3</v>
+      </c>
+      <c r="C33" s="6">
+        <v>3</v>
+      </c>
+      <c r="D33" s="9">
+        <v>5</v>
+      </c>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H33" s="9"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="10"/>
+      <c r="I33" s="11">
+        <v>6</v>
+      </c>
+      <c r="J33" s="11">
+        <v>5</v>
+      </c>
       <c r="K33" s="11"/>
       <c r="L33" s="9"/>
-      <c r="M33" s="11"/>
       <c r="N33" s="9"/>
       <c r="O33" s="9"/>
       <c r="P33" s="9" t="s">
@@ -3788,14 +3767,11 @@
       <c r="Q33" s="9"/>
       <c r="R33" s="7"/>
       <c r="S33" s="7"/>
+      <c r="U33" s="8"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="9">
-        <v>0</v>
-      </c>
+      <c r="A34" s="1"/>
+      <c r="B34" s="9"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
       <c r="E34" s="9"/>
@@ -3803,110 +3779,105 @@
       <c r="G34" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="J34" s="9">
-        <v>1</v>
-      </c>
-      <c r="K34" s="10">
-        <v>1</v>
-      </c>
-      <c r="L34" s="10">
-        <v>1</v>
-      </c>
-      <c r="M34" s="11">
-        <v>1</v>
-      </c>
-      <c r="N34" s="10">
-        <v>0</v>
-      </c>
-      <c r="O34" s="6">
-        <v>1</v>
-      </c>
+      <c r="H34" s="9"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
       <c r="P34" s="9" t="s">
         <v>1</v>
       </c>
       <c r="Q34" s="9"/>
-      <c r="R34" s="7">
-        <v>1</v>
-      </c>
-      <c r="S34" s="7">
-        <v>1</v>
-      </c>
-      <c r="X34" s="6">
-        <v>0</v>
-      </c>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="B35" s="9">
+        <v>0</v>
+      </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>J35&gt;</v>
-      </c>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>M35&gt;</v>
-      </c>
-      <c r="N35" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>N35&gt;</v>
-      </c>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
+      <c r="G35" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J35" s="9">
+        <v>1</v>
+      </c>
+      <c r="K35" s="10">
+        <v>1</v>
+      </c>
+      <c r="L35" s="10">
+        <v>1</v>
+      </c>
+      <c r="M35" s="11">
+        <v>1</v>
+      </c>
+      <c r="N35" s="10">
+        <v>0</v>
+      </c>
+      <c r="O35" s="6">
+        <v>1</v>
+      </c>
+      <c r="P35" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="Q35" s="9"/>
-      <c r="R35" s="7"/>
-      <c r="S35" s="7"/>
+      <c r="R35" s="7">
+        <v>1</v>
+      </c>
+      <c r="S35" s="7">
+        <v>1</v>
+      </c>
+      <c r="X35" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" s="9">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B36" s="9"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
-      <c r="G36" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="J36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>J36&gt;</v>
+      </c>
       <c r="K36" s="10"/>
       <c r="L36" s="10"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="10"/>
-      <c r="P36" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="M36" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>M36&gt;</v>
+      </c>
+      <c r="N36" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>N36&gt;</v>
+      </c>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
       <c r="Q36" s="9"/>
       <c r="R36" s="7"/>
-      <c r="S36" s="7">
-        <v>0</v>
-      </c>
-      <c r="T36" s="6">
-        <v>1</v>
-      </c>
-      <c r="X36" s="6">
-        <v>0</v>
-      </c>
+      <c r="S36" s="7"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="B37" s="9">
+        <v>1</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
@@ -3915,350 +3886,376 @@
       <c r="G37" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="J37" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="K37" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="L37" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="M37" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="N37" s="11" t="s">
+      <c r="J37" s="9"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="10"/>
+      <c r="P37" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7">
         <v>0</v>
       </c>
-      <c r="O37" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P37" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q37" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="R37" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="S37" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="U37" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="V37" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="W37" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="X37" s="6" t="s">
-        <v>6</v>
+      <c r="T37" s="6">
+        <v>1</v>
+      </c>
+      <c r="X37" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B38" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>J38&gt;</v>
-      </c>
-      <c r="K38" s="11"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>M38&gt;</v>
-      </c>
-      <c r="N38" s="11"/>
-      <c r="O38" s="9"/>
-      <c r="P38" s="9"/>
-      <c r="Q38" s="7"/>
-      <c r="R38" s="7"/>
-      <c r="S38" s="7"/>
+      <c r="G38" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="K38" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="L38" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="M38" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="N38" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="O38" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P38" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="R38" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="S38" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="U38" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="V38" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="W38" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="X38" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>22</v>
+      <c r="A39" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
-      <c r="G39" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
       <c r="I39" s="9"/>
-      <c r="J39" s="9">
-        <v>6</v>
-      </c>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
-      <c r="N39" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="O39" s="10">
-        <v>5</v>
-      </c>
-      <c r="P39" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="12"/>
-      <c r="S39" s="12"/>
-      <c r="X39" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="J39" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>J39&gt;</v>
+      </c>
+      <c r="K39" s="11"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>M39&gt;</v>
+      </c>
+      <c r="N39" s="11"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
+      <c r="G40" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="I40" s="9"/>
-      <c r="J40" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>J40&gt;</v>
+      <c r="J40" s="9">
+        <v>6</v>
       </c>
       <c r="K40" s="9"/>
       <c r="L40" s="9"/>
-      <c r="M40" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>M40&gt;</v>
-      </c>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="O40" s="10">
+        <v>5</v>
+      </c>
+      <c r="P40" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="Q40" s="10"/>
       <c r="R40" s="12"/>
       <c r="S40" s="12"/>
+      <c r="X40" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>6</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B41" s="9"/>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
-      <c r="E41" s="11"/>
+      <c r="E41" s="9"/>
       <c r="F41" s="9"/>
-      <c r="G41" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H41" s="9"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
       <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
+      <c r="J41" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>J41&gt;</v>
+      </c>
       <c r="K41" s="9"/>
       <c r="L41" s="9"/>
-      <c r="M41" s="9">
-        <v>1</v>
-      </c>
-      <c r="N41" s="11">
+      <c r="M41" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>M41&gt;</v>
+      </c>
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="10"/>
+      <c r="R41" s="12"/>
+      <c r="S41" s="12"/>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9">
+        <v>1</v>
+      </c>
+      <c r="N42" s="11">
         <v>0</v>
       </c>
-      <c r="O41" s="10"/>
-      <c r="P41" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q41" s="10"/>
-      <c r="R41" s="12">
-        <v>1</v>
-      </c>
-      <c r="S41" s="12">
+      <c r="O42" s="10"/>
+      <c r="P42" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="12">
+        <v>1</v>
+      </c>
+      <c r="S42" s="12">
         <v>0</v>
       </c>
-      <c r="W41" s="6">
-        <v>1</v>
-      </c>
-      <c r="X41" s="6">
+      <c r="W42" s="6">
+        <v>1</v>
+      </c>
+      <c r="X42" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>I42&gt;</v>
-      </c>
-      <c r="J42" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>J42&gt;</v>
-      </c>
-      <c r="K42" s="10"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>M42&gt;</v>
-      </c>
-      <c r="N42" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>N42&gt;</v>
-      </c>
-      <c r="O42" s="11"/>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="9"/>
-      <c r="R42" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>R42&gt;</v>
-      </c>
-      <c r="S42" s="7"/>
-      <c r="W42" s="11" t="str">
-        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
-        <v>W42&gt;</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
-      <c r="N43" s="9"/>
-      <c r="O43" s="9"/>
-      <c r="P43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>I43&gt;</v>
+      </c>
+      <c r="J43" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>J43&gt;</v>
+      </c>
+      <c r="K43" s="10"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>M43&gt;</v>
+      </c>
+      <c r="N43" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>N43&gt;</v>
+      </c>
+      <c r="O43" s="11"/>
+      <c r="P43" s="10"/>
       <c r="Q43" s="9"/>
-      <c r="R43" s="7"/>
+      <c r="R43" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>R43&gt;</v>
+      </c>
       <c r="S43" s="7"/>
-    </row>
-    <row r="44" spans="1:25" s="3" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="13"/>
-      <c r="O44" s="13"/>
-      <c r="P44" s="13"/>
-      <c r="Q44" s="13"/>
-    </row>
-    <row r="45" spans="1:25" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="16" t="s">
+      <c r="W43" s="11" t="str">
+        <f>CONCATENATE(CHAR(COLUMN()+64)&amp;ROW(),"&gt;")</f>
+        <v>W43&gt;</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9"/>
+      <c r="O44" s="9"/>
+      <c r="P44" s="9"/>
+      <c r="Q44" s="9"/>
+      <c r="R44" s="7"/>
+      <c r="S44" s="7"/>
+    </row>
+    <row r="45" spans="1:25" s="3" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="13"/>
+      <c r="O45" s="13"/>
+      <c r="P45" s="13"/>
+      <c r="Q45" s="13"/>
+    </row>
+    <row r="46" spans="1:25" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B46" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C46" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="17"/>
-      <c r="K45" s="17"/>
-      <c r="L45" s="17"/>
-      <c r="M45" s="17"/>
-      <c r="N45" s="17"/>
-      <c r="O45" s="17"/>
-      <c r="P45" s="17"/>
-      <c r="Q45" s="17"/>
-      <c r="R45" s="18"/>
-      <c r="S45" s="18"/>
-      <c r="T45" s="18"/>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A46" s="5"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="7"/>
-      <c r="P46" s="7"/>
-      <c r="Q46" s="7"/>
-      <c r="R46" s="7"/>
-      <c r="S46" s="7"/>
-      <c r="T46" s="7"/>
-      <c r="U46" s="7"/>
-      <c r="V46" s="7"/>
-      <c r="W46" s="7"/>
-      <c r="X46" s="7"/>
-      <c r="Y46" s="7"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="17"/>
+      <c r="O46" s="17"/>
+      <c r="P46" s="17"/>
+      <c r="Q46" s="17"/>
+      <c r="R46" s="18"/>
+      <c r="S46" s="18"/>
+      <c r="T46" s="18"/>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" s="6" t="str">
-        <f>H12</f>
-        <v>H12&gt;</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="A47" s="5"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
+      <c r="Q47" s="7"/>
+      <c r="R47" s="7"/>
+      <c r="S47" s="7"/>
+      <c r="T47" s="7"/>
+      <c r="U47" s="7"/>
+      <c r="V47" s="7"/>
+      <c r="W47" s="7"/>
+      <c r="X47" s="7"/>
+      <c r="Y47" s="7"/>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B48" s="6" t="str">
-        <f>E12</f>
-        <v>E12&gt;</v>
+        <f>H13</f>
+        <v>H13&gt;</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B49" s="6" t="str">
+        <f>E13</f>
+        <v>E13&gt;</v>
+      </c>
       <c r="C49" s="6" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -4266,7 +4263,7 @@
         <v>2</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -4274,203 +4271,192 @@
         <v>2</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="6" t="str">
-        <f>I42</f>
-        <v>I42&gt;</v>
-      </c>
       <c r="C52" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="6" t="str">
+        <f>I43</f>
+        <v>I43&gt;</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="H52" s="6" t="s">
+      <c r="H53" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="3" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-    </row>
-    <row r="56" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="16" t="s">
+    <row r="56" spans="1:8" s="3" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B56" s="19" t="s">
+      <c r="B57" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C56" s="19" t="s">
+      <c r="C57" s="19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="3" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+    <row r="58" spans="1:8" s="3" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C57" s="3" t="str">
-        <f>A4</f>
+      <c r="C58" s="3" t="str">
+        <f>A5</f>
         <v>C50:nclk_a</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="22" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="21"/>
-    </row>
-    <row r="59" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="16" t="s">
+    <row r="59" spans="1:8" s="22" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="21"/>
+    </row>
+    <row r="60" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B59" s="19" t="s">
+      <c r="B60" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D59" s="23"/>
-      <c r="E59" s="23"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C60" s="6" t="str">
-        <f>H8</f>
-        <v>H8&gt;</v>
-      </c>
-      <c r="D60" s="6" t="str">
-        <f>H10</f>
-        <v>H10&gt;</v>
-      </c>
-      <c r="E60" s="6" t="str">
-        <f>H12</f>
-        <v>H12&gt;</v>
-      </c>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C61" s="6" t="str">
-        <f>H10</f>
-        <v>H10&gt;</v>
+        <f>H9</f>
+        <v>H9&gt;</v>
       </c>
       <c r="D61" s="6" t="str">
-        <f>N16</f>
-        <v>N16&gt;</v>
+        <f>H11</f>
+        <v>H11&gt;</v>
       </c>
       <c r="E61" s="6" t="str">
-        <f>R23</f>
-        <v>R23&gt;</v>
+        <f>H13</f>
+        <v>H13&gt;</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C62" s="6" t="str">
-        <f>I23</f>
-        <v>I23&gt;</v>
+        <f>H11</f>
+        <v>H11&gt;</v>
       </c>
       <c r="D62" s="6" t="str">
-        <f>M23</f>
-        <v>M23&gt;</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>27</v>
+        <f>N17</f>
+        <v>N17&gt;</v>
+      </c>
+      <c r="E62" s="6" t="str">
+        <f>R24</f>
+        <v>R24&gt;</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C63" s="6" t="str">
-        <f>J16</f>
-        <v>J16&gt;</v>
+        <f>I24</f>
+        <v>I24&gt;</v>
       </c>
       <c r="D63" s="6" t="str">
-        <f>J19</f>
-        <v>J19&gt;</v>
+        <f>M24</f>
+        <v>M24&gt;</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C64" s="6" t="str">
-        <f>M23</f>
-        <v>M23&gt;</v>
+        <f>J17</f>
+        <v>J17&gt;</v>
       </c>
       <c r="D64" s="6" t="str">
-        <f>M21</f>
-        <v>M21&gt;</v>
-      </c>
-      <c r="E64" s="6" t="str">
-        <f>M19</f>
-        <v>M19&gt;</v>
-      </c>
-      <c r="F64" s="6" t="str">
-        <f>M16</f>
-        <v>M16&gt;</v>
+        <f>J20</f>
+        <v>J20&gt;</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>59</v>
       </c>
       <c r="C65" s="6" t="str">
-        <f>J16</f>
-        <v>J16&gt;</v>
+        <f>M24</f>
+        <v>M24&gt;</v>
       </c>
       <c r="D65" s="6" t="str">
-        <f>J19</f>
-        <v>J19&gt;</v>
+        <f>M22</f>
+        <v>M22&gt;</v>
       </c>
       <c r="E65" s="6" t="str">
-        <f>J21</f>
-        <v>J21&gt;</v>
+        <f>M20</f>
+        <v>M20&gt;</v>
       </c>
       <c r="F65" s="6" t="str">
-        <f>J23</f>
-        <v>J23&gt;</v>
+        <f>M17</f>
+        <v>M17&gt;</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C66" s="6" t="str">
-        <f>N23</f>
-        <v>N23&gt;</v>
+        <f>J17</f>
+        <v>J17&gt;</v>
       </c>
       <c r="D66" s="6" t="str">
-        <f>R23</f>
-        <v>R23&gt;</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>30</v>
+        <f>J20</f>
+        <v>J20&gt;</v>
+      </c>
+      <c r="E66" s="6" t="str">
+        <f>J22</f>
+        <v>J22&gt;</v>
+      </c>
+      <c r="F66" s="6" t="str">
+        <f>J24</f>
+        <v>J24&gt;</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -4481,15 +4467,15 @@
         <v>58</v>
       </c>
       <c r="C67" s="6" t="str">
-        <f>R23</f>
-        <v>R23&gt;</v>
+        <f>N24</f>
+        <v>N24&gt;</v>
       </c>
       <c r="D67" s="6" t="str">
-        <f>W23</f>
-        <v>W23&gt;</v>
+        <f>R24</f>
+        <v>R24&gt;</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -4500,378 +4486,397 @@
         <v>58</v>
       </c>
       <c r="C68" s="6" t="str">
-        <f>R23</f>
-        <v>R23&gt;</v>
+        <f>R24</f>
+        <v>R24&gt;</v>
       </c>
       <c r="D68" s="6" t="str">
-        <f>W23</f>
-        <v>W23&gt;</v>
+        <f>W24</f>
+        <v>W24&gt;</v>
       </c>
       <c r="E68" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C69" s="6" t="str">
+        <f>R24</f>
+        <v>R24&gt;</v>
+      </c>
+      <c r="D69" s="6" t="str">
+        <f>W24</f>
+        <v>W24&gt;</v>
+      </c>
+      <c r="E69" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="3" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
+    <row r="70" spans="1:6" s="3" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">
-    <mergeCell ref="B1:Y1"/>
+    <mergeCell ref="B2:Y2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A47:A55 A59:B59 A15:F21 J14 A12:B14 D13:F13 E14:F14 A22:D22 F22 A60:A66 I44:L44 J18 L18:M18 I20:O20 O14 O22 J15:N15 A11:F11 L4 A4:B4 P4:P7 N11:O13 L11:L14 G4:G7 P9 I8:P8 I10:P10 G9 G11:G21 I22:M22 O23:Q25 K23:L25 J17:N17 K16:L16 K21:L21 S23:V25 N21:O21 L19 F12 C12:D12 H16:I16 H19:I19 H21:I21 A23:H25 O16 O19 P11 I11:J12 C47:XFD55 C64:XFD66 A45:XFD46 N44:XFD44 A2:XFD2 I43:XFD43 Q4:XFD10 P12:XFD22 D60:XFD63 X23:XFD25 R11:XFD11 A56:XFD58 A1:B1 Z1:XFD1 A43:G44 I3:XFD3 A3:G3 D4:F4 C4:C5 A67:XFD1048576">
+  <conditionalFormatting sqref="A48:A56 A60:B60 A16:F22 J15 A13:B15 D14:F14 E15:F15 A23:D23 F23 A61:A67 I45:L45 J19 L19:M19 I21:O21 O15 O23 J16:N16 A12:F12 L5 A5:B5 P5:P8 N12:O14 L12:L15 G5:G8 P10 I9:P9 I11:P11 G10 G12:G22 I23:M23 O24:Q26 K24:L26 J18:N18 K17:L17 K22:L22 S24:V26 N22:O22 L20 F13 C13:D13 H17:I17 H20:I20 H22:I22 A24:H26 O17 O20 P12 I12:J13 C48:XFD56 C65:XFD67 A46:XFD47 N45:XFD45 A3:XFD3 I44:XFD44 Q5:XFD11 P13:XFD23 D61:XFD64 X24:XFD26 R12:XFD12 A57:XFD59 A2:B2 Z2:XFD2 A44:G45 I4:XFD4 A4:G4 D5:F5 C5:C6 A68:XFD1048576">
     <cfRule type="expression" dxfId="70" priority="124">
-      <formula>$A1="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59:XFD59">
+      <formula>$A2="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60:XFD60">
     <cfRule type="expression" dxfId="69" priority="126">
       <formula>#REF!="M:"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K13:K14">
+  <conditionalFormatting sqref="K14:K15">
     <cfRule type="expression" dxfId="68" priority="120">
+      <formula>$A14="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14">
+    <cfRule type="expression" dxfId="67" priority="103">
+      <formula>$A14="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:I15">
+    <cfRule type="expression" dxfId="66" priority="102">
+      <formula>$A14="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
+    <cfRule type="expression" dxfId="65" priority="93">
       <formula>$A13="M:"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J13">
-    <cfRule type="expression" dxfId="67" priority="103">
+  <conditionalFormatting sqref="D15">
+    <cfRule type="expression" dxfId="64" priority="92">
+      <formula>$A15="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="expression" dxfId="63" priority="91">
+      <formula>$A23="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="expression" dxfId="62" priority="83">
       <formula>$A13="M:"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13:I14">
-    <cfRule type="expression" dxfId="66" priority="102">
+  <conditionalFormatting sqref="M45">
+    <cfRule type="expression" dxfId="61" priority="77">
+      <formula>$A45="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M13">
+    <cfRule type="expression" dxfId="60" priority="76">
       <formula>$A13="M:"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12">
-    <cfRule type="expression" dxfId="65" priority="93">
-      <formula>$A12="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="64" priority="92">
-      <formula>$A14="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
-    <cfRule type="expression" dxfId="63" priority="91">
+  <conditionalFormatting sqref="C15">
+    <cfRule type="expression" dxfId="59" priority="75">
+      <formula>$A15="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="expression" dxfId="58" priority="73">
+      <formula>$A15="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="expression" dxfId="57" priority="72">
+      <formula>$A23="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H45">
+    <cfRule type="expression" dxfId="56" priority="65">
+      <formula>$A45="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19:K20">
+    <cfRule type="expression" dxfId="55" priority="61">
+      <formula>$A19="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M15">
+    <cfRule type="expression" dxfId="54" priority="59">
+      <formula>$A15="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N19:N20">
+    <cfRule type="expression" dxfId="53" priority="58">
+      <formula>$A19="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N23">
+    <cfRule type="expression" dxfId="52" priority="55">
+      <formula>$A23="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N15">
+    <cfRule type="expression" dxfId="51" priority="53">
+      <formula>$A15="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:F11 G9 G11 A6:B6 D6:F6">
+    <cfRule type="expression" dxfId="50" priority="52">
+      <formula>$A6="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="expression" dxfId="49" priority="51">
+      <formula>$A9="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="expression" dxfId="48" priority="50">
+      <formula>$A11="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24:I26">
+    <cfRule type="expression" dxfId="47" priority="48">
+      <formula>$A24="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M24:M26">
+    <cfRule type="expression" dxfId="46" priority="47">
+      <formula>$A24="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17">
+    <cfRule type="expression" dxfId="45" priority="46">
+      <formula>$A17="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J22">
+    <cfRule type="expression" dxfId="44" priority="45">
       <formula>$A22="M:"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K12">
-    <cfRule type="expression" dxfId="62" priority="83">
-      <formula>$A12="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M44">
-    <cfRule type="expression" dxfId="61" priority="77">
-      <formula>$A44="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M12">
-    <cfRule type="expression" dxfId="60" priority="76">
-      <formula>$A12="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="59" priority="75">
-      <formula>$A14="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H14">
-    <cfRule type="expression" dxfId="58" priority="73">
-      <formula>$A14="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
-    <cfRule type="expression" dxfId="57" priority="72">
+  <conditionalFormatting sqref="N17">
+    <cfRule type="expression" dxfId="43" priority="44">
+      <formula>$A17="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M22">
+    <cfRule type="expression" dxfId="42" priority="43">
       <formula>$A22="M:"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H44">
-    <cfRule type="expression" dxfId="56" priority="65">
-      <formula>$A44="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18:K19">
-    <cfRule type="expression" dxfId="55" priority="61">
-      <formula>$A18="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M14">
-    <cfRule type="expression" dxfId="54" priority="59">
-      <formula>$A14="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N18:N19">
-    <cfRule type="expression" dxfId="53" priority="58">
-      <formula>$A18="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N22">
-    <cfRule type="expression" dxfId="52" priority="55">
-      <formula>$A22="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N14">
-    <cfRule type="expression" dxfId="51" priority="53">
-      <formula>$A14="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A6:F10 G8 G10 A5:B5 D5:F5">
-    <cfRule type="expression" dxfId="50" priority="52">
-      <formula>$A5="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="49" priority="51">
-      <formula>$A8="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="48" priority="50">
-      <formula>$A10="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I23:I25">
-    <cfRule type="expression" dxfId="47" priority="48">
-      <formula>$A23="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M23:M25">
-    <cfRule type="expression" dxfId="46" priority="47">
-      <formula>$A23="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J16">
-    <cfRule type="expression" dxfId="45" priority="46">
-      <formula>$A16="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J21">
-    <cfRule type="expression" dxfId="44" priority="45">
-      <formula>$A21="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N16">
-    <cfRule type="expression" dxfId="43" priority="44">
-      <formula>$A16="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M21">
-    <cfRule type="expression" dxfId="42" priority="43">
-      <formula>$A21="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M19">
+  <conditionalFormatting sqref="M20">
     <cfRule type="expression" dxfId="41" priority="42">
-      <formula>$A19="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M16">
+      <formula>$A20="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M17">
     <cfRule type="expression" dxfId="40" priority="41">
-      <formula>$A16="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J19">
+      <formula>$A17="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J20">
     <cfRule type="expression" dxfId="39" priority="40">
-      <formula>$A19="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J23:J25">
+      <formula>$A20="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J24:J26">
     <cfRule type="expression" dxfId="38" priority="39">
-      <formula>$A23="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N23:N25">
+      <formula>$A24="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N24:N26">
     <cfRule type="expression" dxfId="37" priority="38">
-      <formula>$A23="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W23:W25">
+      <formula>$A24="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W24:W26">
     <cfRule type="expression" dxfId="36" priority="37">
-      <formula>$A23="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
+      <formula>$A24="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
     <cfRule type="expression" dxfId="35" priority="36">
-      <formula>$A12="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R23:R25">
+      <formula>$A13="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R24:R26">
     <cfRule type="expression" dxfId="34" priority="35">
-      <formula>$A23="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34:F40 J33 A31:B33 D32:F32 E33:F33 A41:D41 F41 J37 L37:M37 I39:O39 O33 O41 J34:N34 A30:F30 P26 N30:O32 L30:L33 G26 P28 I27:P27 I29:P29 G28 G30:G40 I41:M41 O42:Q42 K42:L42 J36:N36 K35:L35 K40:L40 S42:V42 N40:O40 L38 F31 C31:D31 H35:I35 H38:I38 H40:I40 A42:H42 O35 O38 P30 I30:J31 Q26:XFD29 P31:XFD41 X42:XFD42 R30:XFD30">
+      <formula>$A24="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35:F41 J34 A32:B34 D33:F33 E34:F34 A42:D42 F42 J38 L38:M38 I40:O40 O34 O42 J35:N35 A31:F31 P27 N31:O33 L31:L34 G27 P29 I28:P28 I30:P30 G29 G31:G41 I42:M42 O43:Q43 K43:L43 J37:N37 K36:L36 K41:L41 S43:V43 N41:O41 L39 F32 C32:D32 H36:I36 H39:I39 H41:I41 A43:H43 O36 O39 P31 I31:J32 Q27:XFD30 P32:XFD42 X43:XFD43 R31:XFD31">
     <cfRule type="expression" dxfId="33" priority="34">
-      <formula>$A26="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K32:K33">
+      <formula>$A27="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K33:K34">
     <cfRule type="expression" dxfId="32" priority="33">
+      <formula>$A33="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J33">
+    <cfRule type="expression" dxfId="31" priority="32">
+      <formula>$A33="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I33:I34">
+    <cfRule type="expression" dxfId="30" priority="31">
+      <formula>$A33="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32">
+    <cfRule type="expression" dxfId="29" priority="30">
       <formula>$A32="M:"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J32">
-    <cfRule type="expression" dxfId="31" priority="32">
+  <conditionalFormatting sqref="D34">
+    <cfRule type="expression" dxfId="28" priority="29">
+      <formula>$A34="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="expression" dxfId="27" priority="28">
+      <formula>$A42="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K32">
+    <cfRule type="expression" dxfId="26" priority="27">
       <formula>$A32="M:"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32:I33">
-    <cfRule type="expression" dxfId="30" priority="31">
+  <conditionalFormatting sqref="M32">
+    <cfRule type="expression" dxfId="25" priority="26">
       <formula>$A32="M:"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H31">
-    <cfRule type="expression" dxfId="29" priority="30">
-      <formula>$A31="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
-    <cfRule type="expression" dxfId="28" priority="29">
-      <formula>$A33="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
-    <cfRule type="expression" dxfId="27" priority="28">
+  <conditionalFormatting sqref="C34">
+    <cfRule type="expression" dxfId="24" priority="25">
+      <formula>$A34="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34">
+    <cfRule type="expression" dxfId="23" priority="24">
+      <formula>$A34="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H42">
+    <cfRule type="expression" dxfId="22" priority="23">
+      <formula>$A42="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K38:K39">
+    <cfRule type="expression" dxfId="21" priority="22">
+      <formula>$A38="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M34">
+    <cfRule type="expression" dxfId="20" priority="21">
+      <formula>$A34="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N38:N39">
+    <cfRule type="expression" dxfId="19" priority="20">
+      <formula>$A38="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N42">
+    <cfRule type="expression" dxfId="18" priority="19">
+      <formula>$A42="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N34">
+    <cfRule type="expression" dxfId="17" priority="18">
+      <formula>$A34="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:F30 G28 G30">
+    <cfRule type="expression" dxfId="16" priority="17">
+      <formula>$A27="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28">
+    <cfRule type="expression" dxfId="15" priority="16">
+      <formula>$A28="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H30">
+    <cfRule type="expression" dxfId="14" priority="15">
+      <formula>$A30="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I43">
+    <cfRule type="expression" dxfId="13" priority="14">
+      <formula>$A43="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M43">
+    <cfRule type="expression" dxfId="12" priority="13">
+      <formula>$A43="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J36">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>$A36="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J41">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>$A41="M:"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K31">
-    <cfRule type="expression" dxfId="26" priority="27">
-      <formula>$A31="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M31">
-    <cfRule type="expression" dxfId="25" priority="26">
-      <formula>$A31="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C33">
-    <cfRule type="expression" dxfId="24" priority="25">
-      <formula>$A33="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H33">
-    <cfRule type="expression" dxfId="23" priority="24">
-      <formula>$A33="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H41">
-    <cfRule type="expression" dxfId="22" priority="23">
+  <conditionalFormatting sqref="N36">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>$A36="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M41">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>$A41="M:"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K37:K38">
-    <cfRule type="expression" dxfId="21" priority="22">
-      <formula>$A37="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M33">
-    <cfRule type="expression" dxfId="20" priority="21">
-      <formula>$A33="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N37:N38">
-    <cfRule type="expression" dxfId="19" priority="20">
-      <formula>$A37="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N41">
-    <cfRule type="expression" dxfId="18" priority="19">
-      <formula>$A41="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N33">
-    <cfRule type="expression" dxfId="17" priority="18">
-      <formula>$A33="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26:F29 G27 G29">
-    <cfRule type="expression" dxfId="16" priority="17">
-      <formula>$A26="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27">
-    <cfRule type="expression" dxfId="15" priority="16">
-      <formula>$A27="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H29">
-    <cfRule type="expression" dxfId="14" priority="15">
-      <formula>$A29="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
-    <cfRule type="expression" dxfId="13" priority="14">
-      <formula>$A42="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M42">
-    <cfRule type="expression" dxfId="12" priority="13">
-      <formula>$A42="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J35">
-    <cfRule type="expression" dxfId="11" priority="12">
-      <formula>$A35="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J40">
-    <cfRule type="expression" dxfId="10" priority="11">
-      <formula>$A40="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N35">
-    <cfRule type="expression" dxfId="9" priority="10">
-      <formula>$A35="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M40">
-    <cfRule type="expression" dxfId="8" priority="9">
-      <formula>$A40="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M38">
+  <conditionalFormatting sqref="M39">
     <cfRule type="expression" dxfId="7" priority="8">
-      <formula>$A38="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M35">
+      <formula>$A39="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M36">
     <cfRule type="expression" dxfId="6" priority="7">
-      <formula>$A35="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J38">
+      <formula>$A36="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J39">
     <cfRule type="expression" dxfId="5" priority="6">
-      <formula>$A38="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J42">
+      <formula>$A39="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J43">
     <cfRule type="expression" dxfId="4" priority="5">
-      <formula>$A42="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N42">
+      <formula>$A43="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N43">
     <cfRule type="expression" dxfId="3" priority="4">
-      <formula>$A42="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W42">
+      <formula>$A43="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W43">
     <cfRule type="expression" dxfId="2" priority="3">
-      <formula>$A42="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
+      <formula>$A43="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$A31="M:"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R42">
+      <formula>$A32="M:"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R43">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$A42="M:"</formula>
+      <formula>$A43="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
o Changed the font used in waveform label to courier to be fixed widtg than proportional width o changed size of label to script. o Added Gropus, they appear as bold by default. o Corrected forcing of intial condition on buses. Value forced only is cell is empty.
</commit_message>
<xml_diff>
--- a/waveforms__template.xlsx
+++ b/waveforms__template.xlsx
@@ -29,7 +29,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nair Ajayan (IFGB ATV MCD TCD AM):</t>
         </r>
@@ -38,7 +38,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Default is 4:
@@ -58,7 +58,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nair Ajayan (IFGB ATV MCD TCD AM):</t>
         </r>
@@ -67,7 +67,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 o </t>
@@ -101,7 +101,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nair Ajayan (IFGB ATV MCD TCD AM):</t>
         </r>
@@ -110,7 +110,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 o </t>
@@ -137,7 +137,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nair Ajayan (IFGB ATV MCD TCD AM):</t>
         </r>
@@ -146,7 +146,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 o use '|' pipe to indicate a waveform break, discontinutiy in representation. Can be useful for shrnnking waveforms to capture essential info.
@@ -162,7 +162,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nair Ajayan (IFGB ATV MCD TCD AM):</t>
         </r>
@@ -171,7 +171,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Gated clock, Low
@@ -187,7 +187,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nair Ajayan (IFGB ATV MCD TCD AM):</t>
         </r>
@@ -196,7 +196,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 o For legible waveforms which fit into an A4 landscape page, 32 cycles are reccomended. 
@@ -213,7 +213,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nair Ajayan (IFGB ATV MCD TCD AM):</t>
         </r>
@@ -222,7 +222,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 negative clocks
@@ -240,7 +240,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nair Ajayan (IFGB ATV MCD TCD AM):</t>
         </r>
@@ -249,7 +249,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 gated negative clock, High
@@ -265,7 +265,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nair Ajayan (IFGB ATV MCD TCD AM):</t>
         </r>
@@ -274,7 +274,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -308,7 +308,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nair Ajayan (IFGB ATV MCD TCD AM):</t>
         </r>
@@ -317,7 +317,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -350,7 +350,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Nair Ajayan (IFGB ATV MCD TCD AM):
 </t>
@@ -484,7 +484,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nair Ajayan (IFGB ATV MCD TCD AM):</t>
         </r>
@@ -493,7 +493,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 W/o Label node the note is considered  a continulation if marked ith NOTE
@@ -510,7 +510,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nair Ajayan (IFGB ATV MCD TCD AM):</t>
         </r>
@@ -623,7 +623,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="74">
   <si>
     <t>x</t>
   </si>
@@ -836,13 +836,22 @@
   </si>
   <si>
     <t>:SCALE:</t>
+  </si>
+  <si>
+    <t>G:ADDR_CH</t>
+  </si>
+  <si>
+    <t>G:RD_DATA_CH</t>
+  </si>
+  <si>
+    <t>G:Duplication</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
@@ -854,19 +863,6 @@
       <color rgb="FF242729"/>
       <name val="Courier New"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -2497,7 +2493,9 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:Y70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2864,6 +2862,9 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -3114,7 +3115,9 @@
       <c r="U14" s="8"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="B15" s="9"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
@@ -3512,7 +3515,9 @@
       <c r="W25" s="34"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>

</xml_diff>

<commit_message>
o Make consistant fonts o NOTES, Text annotation everything changed to ttfamily.
</commit_message>
<xml_diff>
--- a/waveforms__template.xlsx
+++ b/waveforms__template.xlsx
@@ -623,7 +623,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="75">
   <si>
     <t>x</t>
   </si>
@@ -845,6 +845,9 @@
   </si>
   <si>
     <t>G:Duplication</t>
+  </si>
+  <si>
+    <t>fits08Ch</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1203,117 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="71">
+  <dxfs count="81">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2491,10 +2604,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:Y70"/>
+  <dimension ref="A1:AG70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2503,7 +2616,7 @@
     <col min="2" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>70</v>
       </c>
@@ -2511,7 +2624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>44</v>
       </c>
@@ -2542,7 +2655,7 @@
       <c r="X2" s="35"/>
       <c r="Y2" s="35"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="25"/>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
@@ -2569,7 +2682,7 @@
       <c r="X3" s="24"/>
       <c r="Y3" s="24"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>69</v>
       </c>
@@ -2665,8 +2778,40 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z4" s="6">
+        <f t="shared" ref="Z4:Z6" si="3">Y4+1</f>
+        <v>31</v>
+      </c>
+      <c r="AA4" s="6">
+        <f t="shared" ref="AA4:AA6" si="4">Z4+1</f>
+        <v>32</v>
+      </c>
+      <c r="AB4" s="6">
+        <f t="shared" ref="AB4:AB6" si="5">AA4+1</f>
+        <v>33</v>
+      </c>
+      <c r="AC4" s="6">
+        <f t="shared" ref="AC4:AC6" si="6">AB4+1</f>
+        <v>34</v>
+      </c>
+      <c r="AD4" s="6">
+        <f t="shared" ref="AD4:AD6" si="7">AC4+1</f>
+        <v>35</v>
+      </c>
+      <c r="AE4" s="6">
+        <f t="shared" ref="AE4:AE6" si="8">AD4+1</f>
+        <v>36</v>
+      </c>
+      <c r="AF4" s="6">
+        <f>AE4+1</f>
+        <v>37</v>
+      </c>
+      <c r="AG4" s="6">
+        <f>AF4+1</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2735,35 +2880,67 @@
         <v>22</v>
       </c>
       <c r="S5" s="6">
-        <f t="shared" ref="S5:Y6" si="3">R5+1</f>
+        <f t="shared" ref="S5:Y6" si="9">R5+1</f>
         <v>23</v>
       </c>
       <c r="T5" s="6">
+        <f t="shared" si="9"/>
+        <v>24</v>
+      </c>
+      <c r="U5" s="6">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+      <c r="V5" s="6">
+        <f t="shared" si="9"/>
+        <v>26</v>
+      </c>
+      <c r="W5" s="6">
+        <f t="shared" si="9"/>
+        <v>27</v>
+      </c>
+      <c r="X5" s="6">
+        <f t="shared" si="9"/>
+        <v>28</v>
+      </c>
+      <c r="Y5" s="6">
+        <f t="shared" si="9"/>
+        <v>29</v>
+      </c>
+      <c r="Z5" s="6">
         <f t="shared" si="3"/>
-        <v>24</v>
-      </c>
-      <c r="U5" s="6">
-        <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="V5" s="6">
-        <f t="shared" si="3"/>
-        <v>26</v>
-      </c>
-      <c r="W5" s="6">
-        <f t="shared" si="3"/>
-        <v>27</v>
-      </c>
-      <c r="X5" s="6">
-        <f t="shared" si="3"/>
-        <v>28</v>
-      </c>
-      <c r="Y5" s="6">
-        <f t="shared" si="3"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="AA5" s="6">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="AB5" s="6">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="AC5" s="6">
+        <f t="shared" si="6"/>
+        <v>33</v>
+      </c>
+      <c r="AD5" s="6">
+        <f t="shared" si="7"/>
+        <v>34</v>
+      </c>
+      <c r="AE5" s="6">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="AF5" s="6">
+        <f>AE5+1</f>
+        <v>36</v>
+      </c>
+      <c r="AG5" s="6">
+        <f>AF5+1</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -2798,27 +2975,27 @@
         <v>13</v>
       </c>
       <c r="J6" s="6">
-        <f t="shared" ref="J6" si="4">I6+1</f>
+        <f t="shared" ref="J6" si="10">I6+1</f>
         <v>14</v>
       </c>
       <c r="K6" s="6">
-        <f t="shared" ref="K6" si="5">J6+1</f>
+        <f t="shared" ref="K6" si="11">J6+1</f>
         <v>15</v>
       </c>
       <c r="L6" s="6">
-        <f t="shared" ref="L6" si="6">K6+1</f>
+        <f t="shared" ref="L6" si="12">K6+1</f>
         <v>16</v>
       </c>
       <c r="M6" s="6">
-        <f t="shared" ref="M6" si="7">L6+1</f>
+        <f t="shared" ref="M6" si="13">L6+1</f>
         <v>17</v>
       </c>
       <c r="N6" s="6">
-        <f t="shared" ref="N6" si="8">M6+1</f>
+        <f t="shared" ref="N6" si="14">M6+1</f>
         <v>18</v>
       </c>
       <c r="O6" s="6">
-        <f t="shared" ref="O6" si="9">N6+1</f>
+        <f t="shared" ref="O6" si="15">N6+1</f>
         <v>19</v>
       </c>
       <c r="P6" s="9" t="s">
@@ -2833,35 +3010,67 @@
         <v>23</v>
       </c>
       <c r="S6" s="6">
+        <f t="shared" si="9"/>
+        <v>24</v>
+      </c>
+      <c r="T6" s="6">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+      <c r="U6" s="6">
+        <f t="shared" si="9"/>
+        <v>26</v>
+      </c>
+      <c r="V6" s="6">
+        <f t="shared" si="9"/>
+        <v>27</v>
+      </c>
+      <c r="W6" s="6">
+        <f t="shared" si="9"/>
+        <v>28</v>
+      </c>
+      <c r="X6" s="6">
+        <f t="shared" si="9"/>
+        <v>29</v>
+      </c>
+      <c r="Y6" s="6">
+        <f t="shared" si="9"/>
+        <v>30</v>
+      </c>
+      <c r="Z6" s="6">
         <f t="shared" si="3"/>
-        <v>24</v>
-      </c>
-      <c r="T6" s="6">
-        <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="U6" s="6">
-        <f t="shared" si="3"/>
-        <v>26</v>
-      </c>
-      <c r="V6" s="6">
-        <f t="shared" si="3"/>
-        <v>27</v>
-      </c>
-      <c r="W6" s="6">
-        <f t="shared" si="3"/>
-        <v>28</v>
-      </c>
-      <c r="X6" s="6">
-        <f t="shared" si="3"/>
-        <v>29</v>
-      </c>
-      <c r="Y6" s="6">
-        <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="AA6" s="6">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="AB6" s="6">
+        <f t="shared" si="5"/>
+        <v>33</v>
+      </c>
+      <c r="AC6" s="6">
+        <f t="shared" si="6"/>
+        <v>34</v>
+      </c>
+      <c r="AD6" s="6">
+        <f t="shared" si="7"/>
+        <v>35</v>
+      </c>
+      <c r="AE6" s="6">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+      <c r="AF6" s="6">
+        <f>AE6+1</f>
+        <v>37</v>
+      </c>
+      <c r="AG6" s="6">
+        <f>AF6+1</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>71</v>
       </c>
@@ -2878,7 +3087,7 @@
       </c>
       <c r="Q7" s="9"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -2911,7 +3120,7 @@
       </c>
       <c r="Q8" s="9"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -2935,7 +3144,7 @@
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -2969,7 +3178,7 @@
       </c>
       <c r="Q10" s="9"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -2993,7 +3202,7 @@
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>12</v>
       </c>
@@ -3026,20 +3235,26 @@
         <v>1</v>
       </c>
       <c r="R12" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="S12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="T12" s="8"/>
+        <v>74</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
       <c r="X12" s="6" t="s">
         <v>38</v>
       </c>
       <c r="Y12" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z12" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -3078,7 +3293,7 @@
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -3114,7 +3329,7 @@
       <c r="S14" s="7"/>
       <c r="U14" s="8"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>72</v>
       </c>
@@ -3141,7 +3356,7 @@
       <c r="R15" s="7"/>
       <c r="S15" s="7"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -3156,7 +3371,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K16" s="10">
         <v>1</v>
@@ -4529,358 +4744,358 @@
   <mergeCells count="1">
     <mergeCell ref="B2:Y2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A48:A56 A60:B60 A16:F22 J15 A13:B15 D14:F14 E15:F15 A23:D23 F23 A61:A67 I45:L45 J19 L19:M19 I21:O21 O15 O23 J16:N16 A12:F12 L5 A5:B5 P5:P8 N12:O14 L12:L15 G5:G8 P10 I9:P9 I11:P11 G10 G12:G22 I23:M23 O24:Q26 K24:L26 J18:N18 K17:L17 K22:L22 S24:V26 N22:O22 L20 F13 C13:D13 H17:I17 H20:I20 H22:I22 A24:H26 O17 O20 P12 I12:J13 C48:XFD56 C65:XFD67 A46:XFD47 N45:XFD45 A3:XFD3 I44:XFD44 Q5:XFD11 P13:XFD23 D61:XFD64 X24:XFD26 R12:XFD12 A57:XFD59 A2:B2 Z2:XFD2 A44:G45 I4:XFD4 A4:G4 D5:F5 C5:C6 A68:XFD1048576">
-    <cfRule type="expression" dxfId="70" priority="124">
+  <conditionalFormatting sqref="A48:A56 A60:B60 A16:F22 J15 A13:B15 D14:F14 E15:F15 A23:D23 F23 A61:A67 I45:L45 J19 L19:M19 I21:O21 O15 O23 J16:N16 A12:F12 L5 A5:B5 P5:P8 N12:O14 L12:L15 G5:G8 P10 I9:P9 I11:P11 G10 G12:G22 I23:M23 O24:Q26 K24:L26 J18:N18 K17:L17 K22:L22 S24:V26 N22:O22 L20 F13 C13:D13 H17:I17 H20:I20 H22:I22 A24:H26 O17 O20 P12 I12:J13 C48:XFD56 C65:XFD67 A46:XFD47 N45:XFD45 A3:XFD3 I44:XFD44 P13:XFD23 D61:XFD64 X24:XFD26 A57:XFD59 A2:B2 Z2:XFD2 A44:G45 A4:G4 D5:F5 C5:C6 A68:XFD1048576 I4:AF4 Q7:XFD11 Q5:AF6 AG4:XFD6 R12:XFD12">
+    <cfRule type="expression" dxfId="6" priority="124">
       <formula>$A2="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:XFD60">
-    <cfRule type="expression" dxfId="69" priority="126">
+    <cfRule type="expression" dxfId="77" priority="126">
       <formula>#REF!="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:K15">
-    <cfRule type="expression" dxfId="68" priority="120">
+    <cfRule type="expression" dxfId="76" priority="120">
       <formula>$A14="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="expression" dxfId="67" priority="103">
+    <cfRule type="expression" dxfId="75" priority="103">
       <formula>$A14="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:I15">
-    <cfRule type="expression" dxfId="66" priority="102">
+    <cfRule type="expression" dxfId="74" priority="102">
       <formula>$A14="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="expression" dxfId="65" priority="93">
+    <cfRule type="expression" dxfId="73" priority="93">
       <formula>$A13="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="64" priority="92">
+    <cfRule type="expression" dxfId="72" priority="92">
       <formula>$A15="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="expression" dxfId="63" priority="91">
+    <cfRule type="expression" dxfId="71" priority="91">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="expression" dxfId="62" priority="83">
+    <cfRule type="expression" dxfId="70" priority="83">
       <formula>$A13="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M45">
-    <cfRule type="expression" dxfId="61" priority="77">
+    <cfRule type="expression" dxfId="69" priority="77">
       <formula>$A45="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13">
-    <cfRule type="expression" dxfId="60" priority="76">
+    <cfRule type="expression" dxfId="68" priority="76">
       <formula>$A13="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="59" priority="75">
+    <cfRule type="expression" dxfId="67" priority="75">
       <formula>$A15="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="expression" dxfId="58" priority="73">
+    <cfRule type="expression" dxfId="66" priority="73">
       <formula>$A15="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="expression" dxfId="57" priority="72">
+    <cfRule type="expression" dxfId="65" priority="72">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="expression" dxfId="56" priority="65">
+    <cfRule type="expression" dxfId="64" priority="65">
       <formula>$A45="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19:K20">
-    <cfRule type="expression" dxfId="55" priority="61">
+    <cfRule type="expression" dxfId="63" priority="61">
       <formula>$A19="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M15">
-    <cfRule type="expression" dxfId="54" priority="59">
+    <cfRule type="expression" dxfId="62" priority="59">
       <formula>$A15="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19:N20">
-    <cfRule type="expression" dxfId="53" priority="58">
+    <cfRule type="expression" dxfId="61" priority="58">
       <formula>$A19="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N23">
-    <cfRule type="expression" dxfId="52" priority="55">
+    <cfRule type="expression" dxfId="60" priority="55">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15">
-    <cfRule type="expression" dxfId="51" priority="53">
+    <cfRule type="expression" dxfId="59" priority="53">
       <formula>$A15="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:F11 G9 G11 A6:B6 D6:F6">
-    <cfRule type="expression" dxfId="50" priority="52">
+    <cfRule type="expression" dxfId="58" priority="52">
       <formula>$A6="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="49" priority="51">
+    <cfRule type="expression" dxfId="57" priority="51">
       <formula>$A9="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="expression" dxfId="48" priority="50">
+    <cfRule type="expression" dxfId="56" priority="50">
       <formula>$A11="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:I26">
-    <cfRule type="expression" dxfId="47" priority="48">
+    <cfRule type="expression" dxfId="55" priority="48">
       <formula>$A24="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M24:M26">
-    <cfRule type="expression" dxfId="46" priority="47">
+    <cfRule type="expression" dxfId="54" priority="47">
       <formula>$A24="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17">
-    <cfRule type="expression" dxfId="45" priority="46">
+    <cfRule type="expression" dxfId="53" priority="46">
       <formula>$A17="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22">
-    <cfRule type="expression" dxfId="44" priority="45">
+    <cfRule type="expression" dxfId="52" priority="45">
       <formula>$A22="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17">
-    <cfRule type="expression" dxfId="43" priority="44">
+    <cfRule type="expression" dxfId="51" priority="44">
       <formula>$A17="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M22">
-    <cfRule type="expression" dxfId="42" priority="43">
+    <cfRule type="expression" dxfId="50" priority="43">
       <formula>$A22="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M20">
-    <cfRule type="expression" dxfId="41" priority="42">
+    <cfRule type="expression" dxfId="49" priority="42">
       <formula>$A20="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="expression" dxfId="40" priority="41">
+    <cfRule type="expression" dxfId="48" priority="41">
       <formula>$A17="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20">
-    <cfRule type="expression" dxfId="39" priority="40">
+    <cfRule type="expression" dxfId="47" priority="40">
       <formula>$A20="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:J26">
-    <cfRule type="expression" dxfId="38" priority="39">
+    <cfRule type="expression" dxfId="46" priority="39">
       <formula>$A24="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N24:N26">
-    <cfRule type="expression" dxfId="37" priority="38">
+    <cfRule type="expression" dxfId="45" priority="38">
       <formula>$A24="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W24:W26">
-    <cfRule type="expression" dxfId="36" priority="37">
+    <cfRule type="expression" dxfId="44" priority="37">
       <formula>$A24="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="35" priority="36">
+    <cfRule type="expression" dxfId="43" priority="36">
       <formula>$A13="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R24:R26">
-    <cfRule type="expression" dxfId="34" priority="35">
+    <cfRule type="expression" dxfId="42" priority="35">
       <formula>$A24="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:F41 J34 A32:B34 D33:F33 E34:F34 A42:D42 F42 J38 L38:M38 I40:O40 O34 O42 J35:N35 A31:F31 P27 N31:O33 L31:L34 G27 P29 I28:P28 I30:P30 G29 G31:G41 I42:M42 O43:Q43 K43:L43 J37:N37 K36:L36 K41:L41 S43:V43 N41:O41 L39 F32 C32:D32 H36:I36 H39:I39 H41:I41 A43:H43 O36 O39 P31 I31:J32 Q27:XFD30 P32:XFD42 X43:XFD43 R31:XFD31">
-    <cfRule type="expression" dxfId="33" priority="34">
+    <cfRule type="expression" dxfId="41" priority="34">
       <formula>$A27="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33:K34">
-    <cfRule type="expression" dxfId="32" priority="33">
+    <cfRule type="expression" dxfId="40" priority="33">
       <formula>$A33="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33">
-    <cfRule type="expression" dxfId="31" priority="32">
+    <cfRule type="expression" dxfId="39" priority="32">
       <formula>$A33="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:I34">
-    <cfRule type="expression" dxfId="30" priority="31">
+    <cfRule type="expression" dxfId="38" priority="31">
       <formula>$A33="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="expression" dxfId="29" priority="30">
+    <cfRule type="expression" dxfId="37" priority="30">
       <formula>$A32="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="expression" dxfId="28" priority="29">
+    <cfRule type="expression" dxfId="36" priority="29">
       <formula>$A34="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="expression" dxfId="27" priority="28">
+    <cfRule type="expression" dxfId="35" priority="28">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="expression" dxfId="26" priority="27">
+    <cfRule type="expression" dxfId="34" priority="27">
       <formula>$A32="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="expression" dxfId="25" priority="26">
+    <cfRule type="expression" dxfId="33" priority="26">
       <formula>$A32="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="24" priority="25">
+    <cfRule type="expression" dxfId="32" priority="25">
       <formula>$A34="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="expression" dxfId="23" priority="24">
+    <cfRule type="expression" dxfId="31" priority="24">
       <formula>$A34="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="expression" dxfId="22" priority="23">
+    <cfRule type="expression" dxfId="30" priority="23">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38:K39">
-    <cfRule type="expression" dxfId="21" priority="22">
+    <cfRule type="expression" dxfId="29" priority="22">
       <formula>$A38="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M34">
-    <cfRule type="expression" dxfId="20" priority="21">
+    <cfRule type="expression" dxfId="28" priority="21">
       <formula>$A34="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N38:N39">
-    <cfRule type="expression" dxfId="19" priority="20">
+    <cfRule type="expression" dxfId="27" priority="20">
       <formula>$A38="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N42">
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="26" priority="19">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N34">
-    <cfRule type="expression" dxfId="17" priority="18">
+    <cfRule type="expression" dxfId="25" priority="18">
       <formula>$A34="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:F30 G28 G30">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="24" priority="17">
       <formula>$A27="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="23" priority="16">
       <formula>$A28="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="22" priority="15">
       <formula>$A30="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="21" priority="14">
       <formula>$A43="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M43">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="20" priority="13">
       <formula>$A43="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="19" priority="12">
       <formula>$A36="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="18" priority="11">
       <formula>$A41="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N36">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="17" priority="10">
       <formula>$A36="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M41">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="16" priority="9">
       <formula>$A41="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M39">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="15" priority="8">
       <formula>$A39="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M36">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="14" priority="7">
       <formula>$A36="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="13" priority="6">
       <formula>$A39="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J43">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="12" priority="5">
       <formula>$A43="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N43">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="11" priority="4">
       <formula>$A43="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W43">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>$A43="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>$A32="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R43">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$A43="M:"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
o Enhancement Issue 4. Now use :END: to decide which column to end rendering. o Fixed issue with hardcoded scale on add_grp L o Fixed issue with Tex error in the absense of any NOTEs.
</commit_message>
<xml_diff>
--- a/waveforms__template.xlsx
+++ b/waveforms__template.xlsx
@@ -46,6 +46,32 @@
 @4 approx 22-25 clock cycles can be drawn
 Overflow is indicated by a black box in th PDF.
 Halving scales, for example doubles the clocks that can be drawn
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AF1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nair Ajayan (IFGB ATV MCD TCD AM):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Only draw till this column.
+If not present draw till empty cell.
 </t>
         </r>
       </text>
@@ -623,7 +649,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="76">
   <si>
     <t>x</t>
   </si>
@@ -848,6 +874,9 @@
   </si>
   <si>
     <t>fits08Ch</t>
+  </si>
+  <si>
+    <t>:END:</t>
   </si>
 </sst>
 </file>
@@ -1203,117 +1232,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="81">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="71">
     <dxf>
       <font>
         <strike val="0"/>
@@ -2606,8 +2525,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:AG70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG21" sqref="AG21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2622,6 +2541,9 @@
       </c>
       <c r="B1" s="6">
         <v>4</v>
+      </c>
+      <c r="AF1" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
@@ -2803,11 +2725,11 @@
         <v>36</v>
       </c>
       <c r="AF4" s="6">
-        <f>AE4+1</f>
+        <f t="shared" ref="AF4:AG6" si="9">AE4+1</f>
         <v>37</v>
       </c>
       <c r="AG4" s="6">
-        <f>AF4+1</f>
+        <f t="shared" si="9"/>
         <v>38</v>
       </c>
     </row>
@@ -2880,31 +2802,31 @@
         <v>22</v>
       </c>
       <c r="S5" s="6">
-        <f t="shared" ref="S5:Y6" si="9">R5+1</f>
+        <f t="shared" ref="S5:Y6" si="10">R5+1</f>
         <v>23</v>
       </c>
       <c r="T5" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>24</v>
       </c>
       <c r="U5" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>25</v>
       </c>
       <c r="V5" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>26</v>
       </c>
       <c r="W5" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27</v>
       </c>
       <c r="X5" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>28</v>
       </c>
       <c r="Y5" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>29</v>
       </c>
       <c r="Z5" s="6">
@@ -2932,11 +2854,11 @@
         <v>35</v>
       </c>
       <c r="AF5" s="6">
-        <f>AE5+1</f>
+        <f t="shared" si="9"/>
         <v>36</v>
       </c>
       <c r="AG5" s="6">
-        <f>AF5+1</f>
+        <f t="shared" si="9"/>
         <v>37</v>
       </c>
     </row>
@@ -2975,27 +2897,27 @@
         <v>13</v>
       </c>
       <c r="J6" s="6">
-        <f t="shared" ref="J6" si="10">I6+1</f>
+        <f t="shared" ref="J6" si="11">I6+1</f>
         <v>14</v>
       </c>
       <c r="K6" s="6">
-        <f t="shared" ref="K6" si="11">J6+1</f>
+        <f t="shared" ref="K6" si="12">J6+1</f>
         <v>15</v>
       </c>
       <c r="L6" s="6">
-        <f t="shared" ref="L6" si="12">K6+1</f>
+        <f t="shared" ref="L6" si="13">K6+1</f>
         <v>16</v>
       </c>
       <c r="M6" s="6">
-        <f t="shared" ref="M6" si="13">L6+1</f>
+        <f t="shared" ref="M6" si="14">L6+1</f>
         <v>17</v>
       </c>
       <c r="N6" s="6">
-        <f t="shared" ref="N6" si="14">M6+1</f>
+        <f t="shared" ref="N6" si="15">M6+1</f>
         <v>18</v>
       </c>
       <c r="O6" s="6">
-        <f t="shared" ref="O6" si="15">N6+1</f>
+        <f t="shared" ref="O6" si="16">N6+1</f>
         <v>19</v>
       </c>
       <c r="P6" s="9" t="s">
@@ -3010,31 +2932,31 @@
         <v>23</v>
       </c>
       <c r="S6" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>24</v>
       </c>
       <c r="T6" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>25</v>
       </c>
       <c r="U6" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>26</v>
       </c>
       <c r="V6" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27</v>
       </c>
       <c r="W6" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>28</v>
       </c>
       <c r="X6" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>29</v>
       </c>
       <c r="Y6" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="Z6" s="6">
@@ -3062,11 +2984,11 @@
         <v>36</v>
       </c>
       <c r="AF6" s="6">
-        <f>AE6+1</f>
+        <f t="shared" si="9"/>
         <v>37</v>
       </c>
       <c r="AG6" s="6">
-        <f>AF6+1</f>
+        <f t="shared" si="9"/>
         <v>38</v>
       </c>
     </row>
@@ -4745,357 +4667,357 @@
     <mergeCell ref="B2:Y2"/>
   </mergeCells>
   <conditionalFormatting sqref="A48:A56 A60:B60 A16:F22 J15 A13:B15 D14:F14 E15:F15 A23:D23 F23 A61:A67 I45:L45 J19 L19:M19 I21:O21 O15 O23 J16:N16 A12:F12 L5 A5:B5 P5:P8 N12:O14 L12:L15 G5:G8 P10 I9:P9 I11:P11 G10 G12:G22 I23:M23 O24:Q26 K24:L26 J18:N18 K17:L17 K22:L22 S24:V26 N22:O22 L20 F13 C13:D13 H17:I17 H20:I20 H22:I22 A24:H26 O17 O20 P12 I12:J13 C48:XFD56 C65:XFD67 A46:XFD47 N45:XFD45 A3:XFD3 I44:XFD44 P13:XFD23 D61:XFD64 X24:XFD26 A57:XFD59 A2:B2 Z2:XFD2 A44:G45 A4:G4 D5:F5 C5:C6 A68:XFD1048576 I4:AF4 Q7:XFD11 Q5:AF6 AG4:XFD6 R12:XFD12">
-    <cfRule type="expression" dxfId="6" priority="124">
+    <cfRule type="expression" dxfId="70" priority="124">
       <formula>$A2="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:XFD60">
-    <cfRule type="expression" dxfId="77" priority="126">
+    <cfRule type="expression" dxfId="69" priority="126">
       <formula>#REF!="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:K15">
-    <cfRule type="expression" dxfId="76" priority="120">
+    <cfRule type="expression" dxfId="68" priority="120">
       <formula>$A14="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="expression" dxfId="75" priority="103">
+    <cfRule type="expression" dxfId="67" priority="103">
       <formula>$A14="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:I15">
-    <cfRule type="expression" dxfId="74" priority="102">
+    <cfRule type="expression" dxfId="66" priority="102">
       <formula>$A14="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="expression" dxfId="73" priority="93">
+    <cfRule type="expression" dxfId="65" priority="93">
       <formula>$A13="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="72" priority="92">
+    <cfRule type="expression" dxfId="64" priority="92">
       <formula>$A15="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="expression" dxfId="71" priority="91">
+    <cfRule type="expression" dxfId="63" priority="91">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="expression" dxfId="70" priority="83">
+    <cfRule type="expression" dxfId="62" priority="83">
       <formula>$A13="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M45">
-    <cfRule type="expression" dxfId="69" priority="77">
+    <cfRule type="expression" dxfId="61" priority="77">
       <formula>$A45="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13">
-    <cfRule type="expression" dxfId="68" priority="76">
+    <cfRule type="expression" dxfId="60" priority="76">
       <formula>$A13="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="67" priority="75">
+    <cfRule type="expression" dxfId="59" priority="75">
       <formula>$A15="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="expression" dxfId="66" priority="73">
+    <cfRule type="expression" dxfId="58" priority="73">
       <formula>$A15="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="expression" dxfId="65" priority="72">
+    <cfRule type="expression" dxfId="57" priority="72">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="expression" dxfId="64" priority="65">
+    <cfRule type="expression" dxfId="56" priority="65">
       <formula>$A45="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19:K20">
-    <cfRule type="expression" dxfId="63" priority="61">
+    <cfRule type="expression" dxfId="55" priority="61">
       <formula>$A19="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M15">
-    <cfRule type="expression" dxfId="62" priority="59">
+    <cfRule type="expression" dxfId="54" priority="59">
       <formula>$A15="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19:N20">
-    <cfRule type="expression" dxfId="61" priority="58">
+    <cfRule type="expression" dxfId="53" priority="58">
       <formula>$A19="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N23">
-    <cfRule type="expression" dxfId="60" priority="55">
+    <cfRule type="expression" dxfId="52" priority="55">
       <formula>$A23="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15">
-    <cfRule type="expression" dxfId="59" priority="53">
+    <cfRule type="expression" dxfId="51" priority="53">
       <formula>$A15="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:F11 G9 G11 A6:B6 D6:F6">
-    <cfRule type="expression" dxfId="58" priority="52">
+    <cfRule type="expression" dxfId="50" priority="52">
       <formula>$A6="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="57" priority="51">
+    <cfRule type="expression" dxfId="49" priority="51">
       <formula>$A9="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="expression" dxfId="56" priority="50">
+    <cfRule type="expression" dxfId="48" priority="50">
       <formula>$A11="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:I26">
-    <cfRule type="expression" dxfId="55" priority="48">
+    <cfRule type="expression" dxfId="47" priority="48">
       <formula>$A24="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M24:M26">
-    <cfRule type="expression" dxfId="54" priority="47">
+    <cfRule type="expression" dxfId="46" priority="47">
       <formula>$A24="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17">
-    <cfRule type="expression" dxfId="53" priority="46">
+    <cfRule type="expression" dxfId="45" priority="46">
       <formula>$A17="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22">
-    <cfRule type="expression" dxfId="52" priority="45">
+    <cfRule type="expression" dxfId="44" priority="45">
       <formula>$A22="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17">
-    <cfRule type="expression" dxfId="51" priority="44">
+    <cfRule type="expression" dxfId="43" priority="44">
       <formula>$A17="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M22">
-    <cfRule type="expression" dxfId="50" priority="43">
+    <cfRule type="expression" dxfId="42" priority="43">
       <formula>$A22="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M20">
-    <cfRule type="expression" dxfId="49" priority="42">
+    <cfRule type="expression" dxfId="41" priority="42">
       <formula>$A20="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="expression" dxfId="48" priority="41">
+    <cfRule type="expression" dxfId="40" priority="41">
       <formula>$A17="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20">
-    <cfRule type="expression" dxfId="47" priority="40">
+    <cfRule type="expression" dxfId="39" priority="40">
       <formula>$A20="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:J26">
-    <cfRule type="expression" dxfId="46" priority="39">
+    <cfRule type="expression" dxfId="38" priority="39">
       <formula>$A24="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N24:N26">
-    <cfRule type="expression" dxfId="45" priority="38">
+    <cfRule type="expression" dxfId="37" priority="38">
       <formula>$A24="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W24:W26">
-    <cfRule type="expression" dxfId="44" priority="37">
+    <cfRule type="expression" dxfId="36" priority="37">
       <formula>$A24="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="43" priority="36">
+    <cfRule type="expression" dxfId="35" priority="36">
       <formula>$A13="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R24:R26">
-    <cfRule type="expression" dxfId="42" priority="35">
+    <cfRule type="expression" dxfId="34" priority="35">
       <formula>$A24="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:F41 J34 A32:B34 D33:F33 E34:F34 A42:D42 F42 J38 L38:M38 I40:O40 O34 O42 J35:N35 A31:F31 P27 N31:O33 L31:L34 G27 P29 I28:P28 I30:P30 G29 G31:G41 I42:M42 O43:Q43 K43:L43 J37:N37 K36:L36 K41:L41 S43:V43 N41:O41 L39 F32 C32:D32 H36:I36 H39:I39 H41:I41 A43:H43 O36 O39 P31 I31:J32 Q27:XFD30 P32:XFD42 X43:XFD43 R31:XFD31">
-    <cfRule type="expression" dxfId="41" priority="34">
+    <cfRule type="expression" dxfId="33" priority="34">
       <formula>$A27="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33:K34">
-    <cfRule type="expression" dxfId="40" priority="33">
+    <cfRule type="expression" dxfId="32" priority="33">
       <formula>$A33="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33">
-    <cfRule type="expression" dxfId="39" priority="32">
+    <cfRule type="expression" dxfId="31" priority="32">
       <formula>$A33="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:I34">
-    <cfRule type="expression" dxfId="38" priority="31">
+    <cfRule type="expression" dxfId="30" priority="31">
       <formula>$A33="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="expression" dxfId="37" priority="30">
+    <cfRule type="expression" dxfId="29" priority="30">
       <formula>$A32="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="expression" dxfId="36" priority="29">
+    <cfRule type="expression" dxfId="28" priority="29">
       <formula>$A34="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="expression" dxfId="35" priority="28">
+    <cfRule type="expression" dxfId="27" priority="28">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="expression" dxfId="34" priority="27">
+    <cfRule type="expression" dxfId="26" priority="27">
       <formula>$A32="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="expression" dxfId="33" priority="26">
+    <cfRule type="expression" dxfId="25" priority="26">
       <formula>$A32="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="32" priority="25">
+    <cfRule type="expression" dxfId="24" priority="25">
       <formula>$A34="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="expression" dxfId="31" priority="24">
+    <cfRule type="expression" dxfId="23" priority="24">
       <formula>$A34="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="expression" dxfId="30" priority="23">
+    <cfRule type="expression" dxfId="22" priority="23">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38:K39">
-    <cfRule type="expression" dxfId="29" priority="22">
+    <cfRule type="expression" dxfId="21" priority="22">
       <formula>$A38="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M34">
-    <cfRule type="expression" dxfId="28" priority="21">
+    <cfRule type="expression" dxfId="20" priority="21">
       <formula>$A34="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N38:N39">
-    <cfRule type="expression" dxfId="27" priority="20">
+    <cfRule type="expression" dxfId="19" priority="20">
       <formula>$A38="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N42">
-    <cfRule type="expression" dxfId="26" priority="19">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>$A42="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N34">
-    <cfRule type="expression" dxfId="25" priority="18">
+    <cfRule type="expression" dxfId="17" priority="18">
       <formula>$A34="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:F30 G28 G30">
-    <cfRule type="expression" dxfId="24" priority="17">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>$A27="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="expression" dxfId="23" priority="16">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>$A28="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="expression" dxfId="22" priority="15">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>$A30="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43">
-    <cfRule type="expression" dxfId="21" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>$A43="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M43">
-    <cfRule type="expression" dxfId="20" priority="13">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>$A43="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36">
-    <cfRule type="expression" dxfId="19" priority="12">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>$A36="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41">
-    <cfRule type="expression" dxfId="18" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>$A41="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N36">
-    <cfRule type="expression" dxfId="17" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>$A36="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M41">
-    <cfRule type="expression" dxfId="16" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>$A41="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M39">
-    <cfRule type="expression" dxfId="15" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>$A39="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M36">
-    <cfRule type="expression" dxfId="14" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>$A36="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="expression" dxfId="13" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>$A39="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J43">
-    <cfRule type="expression" dxfId="12" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$A43="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N43">
-    <cfRule type="expression" dxfId="11" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$A43="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W43">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$A43="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$A32="M:"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R43">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$A43="M:"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Issue 5:  Sapacer need to be uniform. Testing and automating this helps reduce design cycles. Implmented methods check_spacers and sanitize_spacers.
Minor:
Chnaged the way groups are displayed. Now rt alligned to make it more visually
consistant.
o Added Signal names to warning associated with missing initial conditions.
</commit_message>
<xml_diff>
--- a/waveforms__template.xlsx
+++ b/waveforms__template.xlsx
@@ -649,7 +649,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="76">
   <si>
     <t>x</t>
   </si>
@@ -2525,8 +2525,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:AG70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG21" sqref="AG21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5:P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2790,9 +2790,7 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="P5" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="P5" s="9"/>
       <c r="Q5" s="9">
         <f>O5+3</f>
         <v>21</v>
@@ -2920,9 +2918,7 @@
         <f t="shared" ref="O6" si="16">N6+1</f>
         <v>19</v>
       </c>
-      <c r="P6" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="P6" s="9"/>
       <c r="Q6" s="9">
         <f>O6+3</f>
         <v>22</v>
@@ -3489,9 +3485,7 @@
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="G21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9">
         <v>6</v>
@@ -3555,9 +3549,6 @@
       <c r="D23" s="9"/>
       <c r="E23" s="11"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -3688,9 +3679,7 @@
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="G27" s="9"/>
       <c r="H27" s="6">
         <v>1</v>
       </c>
@@ -3903,9 +3892,7 @@
       <c r="L33" s="9"/>
       <c r="N33" s="9"/>
       <c r="O33" s="9"/>
-      <c r="P33" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="P33" s="9"/>
       <c r="Q33" s="9"/>
       <c r="R33" s="7"/>
       <c r="S33" s="7"/>
@@ -3929,9 +3916,7 @@
       <c r="M34" s="11"/>
       <c r="N34" s="9"/>
       <c r="O34" s="9"/>
-      <c r="P34" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="P34" s="9"/>
       <c r="Q34" s="9"/>
       <c r="R34" s="7"/>
       <c r="S34" s="7"/>
@@ -3968,9 +3953,7 @@
       <c r="O35" s="6">
         <v>1</v>
       </c>
-      <c r="P35" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="P35" s="9"/>
       <c r="Q35" s="9"/>
       <c r="R35" s="7">
         <v>1</v>
@@ -4033,9 +4016,7 @@
       <c r="L37" s="10"/>
       <c r="M37" s="11"/>
       <c r="N37" s="10"/>
-      <c r="P37" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="P37" s="9"/>
       <c r="Q37" s="9"/>
       <c r="R37" s="7"/>
       <c r="S37" s="7">
@@ -4080,9 +4061,7 @@
       <c r="O38" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P38" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="P38" s="9"/>
       <c r="Q38" s="7" t="s">
         <v>19</v>
       </c>
@@ -4159,9 +4138,7 @@
       <c r="O40" s="10">
         <v>5</v>
       </c>
-      <c r="P40" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="P40" s="9"/>
       <c r="Q40" s="10"/>
       <c r="R40" s="12"/>
       <c r="S40" s="12"/>

</xml_diff>